<commit_message>
added populated dropdowns for the input vaules
</commit_message>
<xml_diff>
--- a/src/main/resources/workbooks/Testing.xlsx
+++ b/src/main/resources/workbooks/Testing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19560" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Test1" sheetId="1" r:id="rId1"/>
@@ -120,10 +120,6 @@
   </si>
   <si>
     <t>Voluntary Cover per month</t>
-  </si>
-  <si>
-    <t>Policy Period Year / 
-ANB</t>
   </si>
   <si>
     <t>All</t>
@@ -238,6 +234,9 @@
   </si>
   <si>
     <t>DTPD</t>
+  </si>
+  <si>
+    <t>Policy Period Year</t>
   </si>
 </sst>
 </file>
@@ -893,87 +892,6 @@
     <xf numFmtId="4" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="6" fontId="3" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1031,15 +949,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -1080,6 +989,96 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1361,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL59"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59:AL59"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1372,263 +1371,263 @@
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
-      <c r="V2" s="44"/>
-      <c r="W2" s="44"/>
-      <c r="X2" s="44"/>
-      <c r="Y2" s="44"/>
-      <c r="Z2" s="45"/>
-      <c r="AA2" s="43" t="s">
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93"/>
+      <c r="S2" s="93"/>
+      <c r="T2" s="93"/>
+      <c r="U2" s="93"/>
+      <c r="V2" s="93"/>
+      <c r="W2" s="93"/>
+      <c r="X2" s="93"/>
+      <c r="Y2" s="93"/>
+      <c r="Z2" s="94"/>
+      <c r="AA2" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="44"/>
-      <c r="AF2" s="44"/>
-      <c r="AG2" s="44"/>
-      <c r="AH2" s="44"/>
-      <c r="AI2" s="44"/>
-      <c r="AJ2" s="44"/>
-      <c r="AK2" s="44"/>
-      <c r="AL2" s="45"/>
+      <c r="AB2" s="93"/>
+      <c r="AC2" s="93"/>
+      <c r="AD2" s="93"/>
+      <c r="AE2" s="93"/>
+      <c r="AF2" s="93"/>
+      <c r="AG2" s="93"/>
+      <c r="AH2" s="93"/>
+      <c r="AI2" s="93"/>
+      <c r="AJ2" s="93"/>
+      <c r="AK2" s="93"/>
+      <c r="AL2" s="94"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="50">
+      <c r="B3" s="95">
         <v>1</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="50"/>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="50"/>
-      <c r="X3" s="50"/>
-      <c r="Y3" s="50"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="95"/>
+      <c r="Q3" s="95"/>
+      <c r="R3" s="95"/>
+      <c r="S3" s="95"/>
+      <c r="T3" s="95"/>
+      <c r="U3" s="95"/>
+      <c r="V3" s="95"/>
+      <c r="W3" s="95"/>
+      <c r="X3" s="95"/>
+      <c r="Y3" s="95"/>
       <c r="Z3" s="2">
         <v>2</v>
       </c>
       <c r="AA3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AB3" s="43" t="s">
+      <c r="AB3" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="AC3" s="44"/>
-      <c r="AD3" s="44"/>
-      <c r="AE3" s="44"/>
-      <c r="AF3" s="44"/>
-      <c r="AG3" s="44"/>
-      <c r="AH3" s="44"/>
-      <c r="AI3" s="44"/>
-      <c r="AJ3" s="44"/>
-      <c r="AK3" s="44"/>
-      <c r="AL3" s="45"/>
+      <c r="AC3" s="93"/>
+      <c r="AD3" s="93"/>
+      <c r="AE3" s="93"/>
+      <c r="AF3" s="93"/>
+      <c r="AG3" s="93"/>
+      <c r="AH3" s="93"/>
+      <c r="AI3" s="93"/>
+      <c r="AJ3" s="93"/>
+      <c r="AK3" s="93"/>
+      <c r="AL3" s="94"/>
     </row>
     <row r="4" spans="1:38" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51" t="s">
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51" t="s">
+      <c r="F4" s="96"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51" t="s">
+      <c r="I4" s="96"/>
+      <c r="J4" s="96"/>
+      <c r="K4" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51" t="s">
+      <c r="L4" s="96"/>
+      <c r="M4" s="96"/>
+      <c r="N4" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="51" t="s">
+      <c r="O4" s="96"/>
+      <c r="P4" s="96"/>
+      <c r="Q4" s="96" t="s">
         <v>11</v>
       </c>
-      <c r="R4" s="51"/>
-      <c r="S4" s="51"/>
-      <c r="T4" s="51" t="s">
+      <c r="R4" s="96"/>
+      <c r="S4" s="96"/>
+      <c r="T4" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="U4" s="51"/>
-      <c r="V4" s="51"/>
-      <c r="W4" s="52" t="s">
+      <c r="U4" s="96"/>
+      <c r="V4" s="96"/>
+      <c r="W4" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="X4" s="53"/>
-      <c r="Y4" s="54"/>
+      <c r="X4" s="98"/>
+      <c r="Y4" s="99"/>
       <c r="Z4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="AA4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="52" t="s">
+      <c r="AB4" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="AC4" s="53"/>
-      <c r="AD4" s="53"/>
-      <c r="AE4" s="53"/>
-      <c r="AF4" s="53"/>
-      <c r="AG4" s="53"/>
-      <c r="AH4" s="53"/>
-      <c r="AI4" s="53"/>
-      <c r="AJ4" s="53"/>
-      <c r="AK4" s="53"/>
-      <c r="AL4" s="54"/>
+      <c r="AC4" s="98"/>
+      <c r="AD4" s="98"/>
+      <c r="AE4" s="98"/>
+      <c r="AF4" s="98"/>
+      <c r="AG4" s="98"/>
+      <c r="AH4" s="98"/>
+      <c r="AI4" s="98"/>
+      <c r="AJ4" s="98"/>
+      <c r="AK4" s="98"/>
+      <c r="AL4" s="99"/>
     </row>
     <row r="5" spans="1:38" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="46"/>
-      <c r="S5" s="46"/>
-      <c r="T5" s="46"/>
-      <c r="U5" s="46"/>
-      <c r="V5" s="46"/>
-      <c r="W5" s="46"/>
-      <c r="X5" s="46"/>
-      <c r="Y5" s="46"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="100"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="100"/>
+      <c r="L5" s="100"/>
+      <c r="M5" s="100"/>
+      <c r="N5" s="100"/>
+      <c r="O5" s="100"/>
+      <c r="P5" s="100"/>
+      <c r="Q5" s="100"/>
+      <c r="R5" s="100"/>
+      <c r="S5" s="100"/>
+      <c r="T5" s="100"/>
+      <c r="U5" s="100"/>
+      <c r="V5" s="100"/>
+      <c r="W5" s="100"/>
+      <c r="X5" s="100"/>
+      <c r="Y5" s="100"/>
       <c r="Z5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="AA5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AB5" s="43" t="s">
+      <c r="AB5" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="AC5" s="44"/>
-      <c r="AD5" s="44"/>
-      <c r="AE5" s="44"/>
-      <c r="AF5" s="44"/>
-      <c r="AG5" s="44"/>
-      <c r="AH5" s="44"/>
-      <c r="AI5" s="44"/>
-      <c r="AJ5" s="44"/>
-      <c r="AK5" s="44"/>
-      <c r="AL5" s="45"/>
+      <c r="AC5" s="93"/>
+      <c r="AD5" s="93"/>
+      <c r="AE5" s="93"/>
+      <c r="AF5" s="93"/>
+      <c r="AG5" s="93"/>
+      <c r="AH5" s="93"/>
+      <c r="AI5" s="93"/>
+      <c r="AJ5" s="93"/>
+      <c r="AK5" s="93"/>
+      <c r="AL5" s="94"/>
     </row>
     <row r="6" spans="1:38" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="43" t="s">
+      <c r="C6" s="93"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="44"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="43" t="s">
+      <c r="F6" s="93"/>
+      <c r="G6" s="94"/>
+      <c r="H6" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="44"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="43" t="s">
+      <c r="I6" s="93"/>
+      <c r="J6" s="94"/>
+      <c r="K6" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="44"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="43" t="s">
+      <c r="L6" s="93"/>
+      <c r="M6" s="94"/>
+      <c r="N6" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="44"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="43" t="s">
+      <c r="O6" s="93"/>
+      <c r="P6" s="94"/>
+      <c r="Q6" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="R6" s="44"/>
-      <c r="S6" s="45"/>
-      <c r="T6" s="43" t="s">
+      <c r="R6" s="93"/>
+      <c r="S6" s="94"/>
+      <c r="T6" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="U6" s="44"/>
-      <c r="V6" s="45"/>
-      <c r="W6" s="43" t="s">
+      <c r="U6" s="93"/>
+      <c r="V6" s="94"/>
+      <c r="W6" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="X6" s="44"/>
-      <c r="Y6" s="45"/>
+      <c r="X6" s="93"/>
+      <c r="Y6" s="94"/>
       <c r="Z6" s="4" t="s">
         <v>20</v>
       </c>
@@ -1673,46 +1672,46 @@
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="43" t="s">
+      <c r="C7" s="93"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="44"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="43" t="s">
+      <c r="F7" s="93"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="44"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="43" t="s">
+      <c r="I7" s="93"/>
+      <c r="J7" s="94"/>
+      <c r="K7" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="44"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="43" t="s">
+      <c r="L7" s="93"/>
+      <c r="M7" s="94"/>
+      <c r="N7" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="44"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="43" t="s">
+      <c r="O7" s="93"/>
+      <c r="P7" s="94"/>
+      <c r="Q7" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="R7" s="44"/>
-      <c r="S7" s="45"/>
-      <c r="T7" s="43" t="s">
+      <c r="R7" s="93"/>
+      <c r="S7" s="94"/>
+      <c r="T7" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="U7" s="44"/>
-      <c r="V7" s="45"/>
-      <c r="W7" s="43" t="s">
+      <c r="U7" s="93"/>
+      <c r="V7" s="94"/>
+      <c r="W7" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="X7" s="44"/>
-      <c r="Y7" s="45"/>
+      <c r="X7" s="93"/>
+      <c r="Y7" s="94"/>
       <c r="Z7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1757,57 +1756,57 @@
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="46"/>
-      <c r="N8" s="46"/>
-      <c r="O8" s="46"/>
-      <c r="P8" s="46"/>
-      <c r="Q8" s="46"/>
-      <c r="R8" s="46"/>
-      <c r="S8" s="46"/>
-      <c r="T8" s="46"/>
-      <c r="U8" s="46"/>
-      <c r="V8" s="46"/>
-      <c r="W8" s="45" t="s">
+      <c r="C8" s="100"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="100"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="100"/>
+      <c r="I8" s="100"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="100"/>
+      <c r="L8" s="100"/>
+      <c r="M8" s="100"/>
+      <c r="N8" s="100"/>
+      <c r="O8" s="100"/>
+      <c r="P8" s="100"/>
+      <c r="Q8" s="100"/>
+      <c r="R8" s="100"/>
+      <c r="S8" s="100"/>
+      <c r="T8" s="100"/>
+      <c r="U8" s="100"/>
+      <c r="V8" s="100"/>
+      <c r="W8" s="94" t="s">
         <v>27</v>
       </c>
-      <c r="X8" s="46"/>
-      <c r="Y8" s="46"/>
+      <c r="X8" s="100"/>
+      <c r="Y8" s="100"/>
       <c r="Z8" s="2" t="s">
         <v>28</v>
       </c>
       <c r="AA8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AB8" s="43" t="s">
+      <c r="AB8" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="AC8" s="44"/>
-      <c r="AD8" s="44"/>
-      <c r="AE8" s="44"/>
-      <c r="AF8" s="44"/>
-      <c r="AG8" s="44"/>
-      <c r="AH8" s="44"/>
-      <c r="AI8" s="44"/>
-      <c r="AJ8" s="44"/>
-      <c r="AK8" s="44"/>
-      <c r="AL8" s="45"/>
-    </row>
-    <row r="9" spans="1:38" ht="30" x14ac:dyDescent="0.2">
+      <c r="AC8" s="93"/>
+      <c r="AD8" s="93"/>
+      <c r="AE8" s="93"/>
+      <c r="AF8" s="93"/>
+      <c r="AG8" s="93"/>
+      <c r="AH8" s="93"/>
+      <c r="AI8" s="93"/>
+      <c r="AJ8" s="93"/>
+      <c r="AK8" s="93"/>
+      <c r="AL8" s="94"/>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
@@ -1882,24 +1881,24 @@
         <v>3</v>
       </c>
       <c r="Z9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB9" s="101" t="s">
         <v>31</v>
       </c>
-      <c r="AA9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB9" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC9" s="48"/>
-      <c r="AD9" s="48"/>
-      <c r="AE9" s="48"/>
-      <c r="AF9" s="48"/>
-      <c r="AG9" s="48"/>
-      <c r="AH9" s="48"/>
-      <c r="AI9" s="48"/>
-      <c r="AJ9" s="48"/>
-      <c r="AK9" s="48"/>
-      <c r="AL9" s="49"/>
+      <c r="AC9" s="102"/>
+      <c r="AD9" s="102"/>
+      <c r="AE9" s="102"/>
+      <c r="AF9" s="102"/>
+      <c r="AG9" s="102"/>
+      <c r="AH9" s="102"/>
+      <c r="AI9" s="102"/>
+      <c r="AJ9" s="102"/>
+      <c r="AK9" s="102"/>
+      <c r="AL9" s="103"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -9601,6 +9600,28 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="W7:Y7"/>
+    <mergeCell ref="B8:V8"/>
+    <mergeCell ref="W8:Y8"/>
+    <mergeCell ref="AB8:AL8"/>
+    <mergeCell ref="AB9:AL9"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="T7:V7"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="B5:Y5"/>
+    <mergeCell ref="AB5:AL5"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="T6:V6"/>
+    <mergeCell ref="W6:Y6"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N6:P6"/>
     <mergeCell ref="B2:Z2"/>
     <mergeCell ref="AA2:AL2"/>
     <mergeCell ref="B3:Y3"/>
@@ -9614,28 +9635,6 @@
     <mergeCell ref="T4:V4"/>
     <mergeCell ref="W4:Y4"/>
     <mergeCell ref="AB4:AL4"/>
-    <mergeCell ref="B5:Y5"/>
-    <mergeCell ref="AB5:AL5"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="T6:V6"/>
-    <mergeCell ref="W6:Y6"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="W7:Y7"/>
-    <mergeCell ref="B8:V8"/>
-    <mergeCell ref="W8:Y8"/>
-    <mergeCell ref="AB8:AL8"/>
-    <mergeCell ref="AB9:AL9"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="T7:V7"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="N7:P7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9653,61 +9652,61 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="104" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>35</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="104" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55" t="s">
+      <c r="E2" s="104"/>
+      <c r="F2" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="E2" s="55"/>
-      <c r="F2" s="13" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
+        <v>45</v>
+      </c>
+      <c r="B4" s="104" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="104"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="104"/>
+      <c r="F4" s="104"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14">
@@ -9834,19 +9833,19 @@
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
       <c r="D2" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2" s="19"/>
-      <c r="F2" s="62" t="s">
+      <c r="F2" s="111" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="33" t="s">
+      <c r="J2" s="34" t="s">
         <v>35</v>
-      </c>
-      <c r="J2" s="34" t="s">
-        <v>36</v>
       </c>
       <c r="K2" s="18"/>
     </row>
@@ -9855,19 +9854,19 @@
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" s="19"/>
-      <c r="F3" s="64" t="s">
+      <c r="F3" s="113" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="114"/>
+      <c r="H3" s="114" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65" t="s">
+      <c r="I3" s="114"/>
+      <c r="J3" s="35" t="s">
         <v>38</v>
-      </c>
-      <c r="I3" s="65"/>
-      <c r="J3" s="35" t="s">
-        <v>39</v>
       </c>
       <c r="K3" s="18"/>
     </row>
@@ -9876,18 +9875,18 @@
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
       <c r="D4" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="114" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="65" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="66"/>
+      <c r="H4" s="114"/>
+      <c r="I4" s="114"/>
+      <c r="J4" s="115"/>
       <c r="K4" s="18"/>
     </row>
     <row r="5" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -9895,28 +9894,28 @@
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="19"/>
-      <c r="F5" s="67" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="69"/>
+      <c r="F5" s="116" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="117"/>
+      <c r="H5" s="117"/>
+      <c r="I5" s="117"/>
+      <c r="J5" s="118"/>
       <c r="K5" s="18"/>
     </row>
     <row r="6" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="D6" s="20" t="s">
         <v>48</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>49</v>
       </c>
       <c r="E6" s="19"/>
       <c r="F6" s="20"/>
@@ -9929,9 +9928,9 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="18"/>
       <c r="B7" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="107" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="38">
@@ -9957,10 +9956,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="18"/>
-      <c r="B8" s="56" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="59"/>
+      <c r="B8" s="105" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="108"/>
       <c r="D8" s="39">
         <v>2</v>
       </c>
@@ -9984,8 +9983,8 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="18"/>
-      <c r="B9" s="57"/>
-      <c r="C9" s="60" t="s">
+      <c r="B9" s="106"/>
+      <c r="C9" s="109" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="39">
@@ -10012,9 +10011,9 @@
     <row r="10" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="61"/>
+        <v>44</v>
+      </c>
+      <c r="C10" s="110"/>
       <c r="D10" s="41">
         <v>4</v>
       </c>
@@ -10068,2646 +10067,2646 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="4" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C4" s="100"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="102"/>
-      <c r="L4" s="100"/>
-      <c r="M4" s="101"/>
-      <c r="N4" s="101"/>
-      <c r="O4" s="101"/>
-      <c r="P4" s="102"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="75"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="74"/>
+      <c r="N4" s="74"/>
+      <c r="O4" s="74"/>
+      <c r="P4" s="75"/>
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C5" s="103" t="s">
+      <c r="C5" s="119" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="120"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="120"/>
+      <c r="G5" s="120"/>
+      <c r="H5" s="120"/>
+      <c r="I5" s="121"/>
+      <c r="L5" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="104"/>
-      <c r="E5" s="104"/>
-      <c r="F5" s="104"/>
-      <c r="G5" s="104"/>
-      <c r="H5" s="104"/>
-      <c r="I5" s="105"/>
-      <c r="L5" s="103" t="s">
+      <c r="M5" s="120"/>
+      <c r="N5" s="120"/>
+      <c r="O5" s="120"/>
+      <c r="P5" s="121"/>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C6" s="76"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="77"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="78"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="77"/>
+      <c r="P6" s="78"/>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C7" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="M5" s="104"/>
-      <c r="N5" s="104"/>
-      <c r="O5" s="104"/>
-      <c r="P5" s="105"/>
-    </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C6" s="106"/>
-      <c r="D6" s="107"/>
-      <c r="E6" s="107"/>
-      <c r="F6" s="107"/>
-      <c r="G6" s="107"/>
-      <c r="H6" s="107"/>
-      <c r="I6" s="108"/>
-      <c r="L6" s="106"/>
-      <c r="M6" s="107"/>
-      <c r="N6" s="107"/>
-      <c r="O6" s="107"/>
-      <c r="P6" s="108"/>
-    </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C7" s="109" t="s">
+      <c r="D7" s="43">
+        <v>10000</v>
+      </c>
+      <c r="E7" s="44">
+        <v>10000</v>
+      </c>
+      <c r="F7" s="44">
+        <v>10000</v>
+      </c>
+      <c r="G7" s="44">
+        <v>10000</v>
+      </c>
+      <c r="H7" s="44">
+        <v>10000</v>
+      </c>
+      <c r="I7" s="45">
+        <v>10000</v>
+      </c>
+      <c r="L7" s="79" t="s">
+        <v>55</v>
+      </c>
+      <c r="M7" s="82">
+        <v>1000</v>
+      </c>
+      <c r="N7" s="83">
+        <v>1000</v>
+      </c>
+      <c r="O7" s="83">
+        <v>1000</v>
+      </c>
+      <c r="P7" s="84">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C8" s="80" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="70">
-        <v>10000</v>
-      </c>
-      <c r="E7" s="71">
-        <v>10000</v>
-      </c>
-      <c r="F7" s="71">
-        <v>10000</v>
-      </c>
-      <c r="G7" s="71">
-        <v>10000</v>
-      </c>
-      <c r="H7" s="71">
-        <v>10000</v>
-      </c>
-      <c r="I7" s="72">
-        <v>10000</v>
-      </c>
-      <c r="L7" s="109" t="s">
-        <v>56</v>
-      </c>
-      <c r="M7" s="112">
-        <v>1000</v>
-      </c>
-      <c r="N7" s="113">
-        <v>1000</v>
-      </c>
-      <c r="O7" s="113">
-        <v>1000</v>
-      </c>
-      <c r="P7" s="114">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C8" s="110" t="s">
+      <c r="D8" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="73" t="s">
+      <c r="E8" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="74" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="74" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="74" t="str">
+      <c r="G8" s="47" t="str">
         <f>F8</f>
         <v>Group 2</v>
       </c>
-      <c r="H8" s="74" t="s">
-        <v>60</v>
-      </c>
-      <c r="I8" s="75" t="str">
+      <c r="H8" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="48" t="str">
         <f>H8</f>
         <v>Group 3</v>
       </c>
-      <c r="L8" s="115" t="s">
+      <c r="L8" s="85" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" s="86" t="s">
         <v>61</v>
       </c>
-      <c r="M8" s="116" t="s">
+      <c r="N8" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="N8" s="117" t="s">
+      <c r="O8" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="O8" s="117" t="s">
+      <c r="P8" s="88" t="s">
         <v>64</v>
       </c>
-      <c r="P8" s="118" t="s">
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C9" s="81" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C9" s="111" t="s">
+      <c r="D9" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="76" t="s">
+      <c r="E9" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="77" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="77" t="s">
+      <c r="F9" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="77" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" s="77" t="s">
+      <c r="H9" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="I9" s="78" t="s">
-        <v>68</v>
-      </c>
-      <c r="L9" s="119">
+      <c r="L9" s="89">
         <v>16</v>
       </c>
-      <c r="M9" s="79">
+      <c r="M9" s="52">
         <v>10</v>
       </c>
-      <c r="N9" s="80">
+      <c r="N9" s="53">
         <f>M9+10</f>
         <v>20</v>
       </c>
-      <c r="O9" s="80">
+      <c r="O9" s="53">
         <f>N9+10</f>
         <v>30</v>
       </c>
-      <c r="P9" s="93">
+      <c r="P9" s="66">
         <f>O9+10</f>
         <v>40</v>
       </c>
     </row>
     <row r="10" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C10" s="81">
+      <c r="C10" s="54">
         <v>16</v>
       </c>
-      <c r="D10" s="82">
+      <c r="D10" s="55">
         <v>1</v>
       </c>
-      <c r="E10" s="83">
+      <c r="E10" s="56">
         <v>2</v>
       </c>
-      <c r="F10" s="83">
+      <c r="F10" s="56">
         <v>3</v>
       </c>
-      <c r="G10" s="83">
+      <c r="G10" s="56">
         <v>4</v>
       </c>
-      <c r="H10" s="83">
+      <c r="H10" s="56">
         <v>5</v>
       </c>
-      <c r="I10" s="84">
+      <c r="I10" s="57">
         <v>6</v>
       </c>
-      <c r="L10" s="120">
+      <c r="L10" s="90">
         <f>L9+1</f>
         <v>17</v>
       </c>
-      <c r="M10" s="94">
+      <c r="M10" s="67">
         <f>M9+2</f>
         <v>12</v>
       </c>
-      <c r="N10" s="95">
+      <c r="N10" s="68">
         <f t="shared" ref="N10:P10" si="0">N9+2</f>
         <v>22</v>
       </c>
-      <c r="O10" s="95">
+      <c r="O10" s="68">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="P10" s="96">
+      <c r="P10" s="69">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
     </row>
     <row r="11" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C11" s="85">
+      <c r="C11" s="58">
         <f>C10+1</f>
         <v>17</v>
       </c>
-      <c r="D11" s="86">
+      <c r="D11" s="59">
         <f>D10+1</f>
         <v>2</v>
       </c>
-      <c r="E11" s="87">
+      <c r="E11" s="60">
         <f t="shared" ref="E11:I59" si="1">E10+1</f>
         <v>3</v>
       </c>
-      <c r="F11" s="87">
+      <c r="F11" s="60">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G11" s="87">
+      <c r="G11" s="60">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="H11" s="87">
+      <c r="H11" s="60">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I11" s="88">
+      <c r="I11" s="61">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="L11" s="120">
+      <c r="L11" s="90">
         <f t="shared" ref="L11:L58" si="2">L10+1</f>
         <v>18</v>
       </c>
-      <c r="M11" s="94">
+      <c r="M11" s="67">
         <f t="shared" ref="M11:M58" si="3">M10+2</f>
         <v>14</v>
       </c>
-      <c r="N11" s="95">
+      <c r="N11" s="68">
         <f t="shared" ref="N11:N58" si="4">N10+2</f>
         <v>24</v>
       </c>
-      <c r="O11" s="95">
+      <c r="O11" s="68">
         <f t="shared" ref="O11:O58" si="5">O10+2</f>
         <v>34</v>
       </c>
-      <c r="P11" s="96">
+      <c r="P11" s="69">
         <f t="shared" ref="P11:P58" si="6">P10+2</f>
         <v>44</v>
       </c>
     </row>
     <row r="12" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C12" s="85">
+      <c r="C12" s="58">
         <f t="shared" ref="C12:D27" si="7">C11+1</f>
         <v>18</v>
       </c>
-      <c r="D12" s="86">
+      <c r="D12" s="59">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="E12" s="87">
+      <c r="E12" s="60">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F12" s="87">
+      <c r="F12" s="60">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="G12" s="87">
+      <c r="G12" s="60">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="H12" s="87">
+      <c r="H12" s="60">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I12" s="88">
+      <c r="I12" s="61">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="L12" s="120">
+      <c r="L12" s="90">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="M12" s="94">
+      <c r="M12" s="67">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="N12" s="95">
+      <c r="N12" s="68">
         <f t="shared" si="4"/>
         <v>26</v>
       </c>
-      <c r="O12" s="95">
+      <c r="O12" s="68">
         <f t="shared" si="5"/>
         <v>36</v>
       </c>
-      <c r="P12" s="96">
+      <c r="P12" s="69">
         <f t="shared" si="6"/>
         <v>46</v>
       </c>
     </row>
     <row r="13" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C13" s="85">
+      <c r="C13" s="58">
         <f t="shared" si="7"/>
         <v>19</v>
       </c>
-      <c r="D13" s="86">
+      <c r="D13" s="59">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="E13" s="87">
+      <c r="E13" s="60">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="F13" s="87">
+      <c r="F13" s="60">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G13" s="87">
+      <c r="G13" s="60">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="H13" s="87">
+      <c r="H13" s="60">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="I13" s="88">
+      <c r="I13" s="61">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="L13" s="120">
+      <c r="L13" s="90">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="M13" s="94">
+      <c r="M13" s="67">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="N13" s="95">
+      <c r="N13" s="68">
         <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="O13" s="95">
+      <c r="O13" s="68">
         <f t="shared" si="5"/>
         <v>38</v>
       </c>
-      <c r="P13" s="96">
+      <c r="P13" s="69">
         <f t="shared" si="6"/>
         <v>48</v>
       </c>
     </row>
     <row r="14" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C14" s="85">
+      <c r="C14" s="58">
         <f t="shared" si="7"/>
         <v>20</v>
       </c>
-      <c r="D14" s="86">
+      <c r="D14" s="59">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="E14" s="87">
+      <c r="E14" s="60">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="F14" s="87">
+      <c r="F14" s="60">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="G14" s="87">
+      <c r="G14" s="60">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="H14" s="87">
+      <c r="H14" s="60">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="I14" s="88">
+      <c r="I14" s="61">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="L14" s="120">
+      <c r="L14" s="90">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="M14" s="94">
+      <c r="M14" s="67">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="N14" s="95">
+      <c r="N14" s="68">
         <f t="shared" si="4"/>
         <v>30</v>
       </c>
-      <c r="O14" s="95">
+      <c r="O14" s="68">
         <f t="shared" si="5"/>
         <v>40</v>
       </c>
-      <c r="P14" s="96">
+      <c r="P14" s="69">
         <f t="shared" si="6"/>
         <v>50</v>
       </c>
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C15" s="85">
+      <c r="C15" s="58">
         <f t="shared" si="7"/>
         <v>21</v>
       </c>
-      <c r="D15" s="86">
+      <c r="D15" s="59">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="E15" s="87">
+      <c r="E15" s="60">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="F15" s="87">
+      <c r="F15" s="60">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="G15" s="87">
+      <c r="G15" s="60">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="H15" s="87">
+      <c r="H15" s="60">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="I15" s="88">
+      <c r="I15" s="61">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="L15" s="120">
+      <c r="L15" s="90">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="M15" s="94">
+      <c r="M15" s="67">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="N15" s="95">
+      <c r="N15" s="68">
         <f t="shared" si="4"/>
         <v>32</v>
       </c>
-      <c r="O15" s="95">
+      <c r="O15" s="68">
         <f t="shared" si="5"/>
         <v>42</v>
       </c>
-      <c r="P15" s="96">
+      <c r="P15" s="69">
         <f t="shared" si="6"/>
         <v>52</v>
       </c>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C16" s="85">
+      <c r="C16" s="58">
         <f t="shared" si="7"/>
         <v>22</v>
       </c>
-      <c r="D16" s="86">
+      <c r="D16" s="59">
         <f t="shared" si="7"/>
         <v>7</v>
       </c>
-      <c r="E16" s="87">
+      <c r="E16" s="60">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="F16" s="87">
+      <c r="F16" s="60">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="G16" s="87">
+      <c r="G16" s="60">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="H16" s="87">
+      <c r="H16" s="60">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="I16" s="88">
+      <c r="I16" s="61">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="L16" s="120">
+      <c r="L16" s="90">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="M16" s="94">
+      <c r="M16" s="67">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="N16" s="95">
+      <c r="N16" s="68">
         <f t="shared" si="4"/>
         <v>34</v>
       </c>
-      <c r="O16" s="95">
+      <c r="O16" s="68">
         <f t="shared" si="5"/>
         <v>44</v>
       </c>
-      <c r="P16" s="96">
+      <c r="P16" s="69">
         <f t="shared" si="6"/>
         <v>54</v>
       </c>
     </row>
     <row r="17" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C17" s="85">
+      <c r="C17" s="58">
         <f t="shared" si="7"/>
         <v>23</v>
       </c>
-      <c r="D17" s="86">
+      <c r="D17" s="59">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="E17" s="87">
+      <c r="E17" s="60">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="F17" s="87">
+      <c r="F17" s="60">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="G17" s="87">
+      <c r="G17" s="60">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="H17" s="87">
+      <c r="H17" s="60">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="I17" s="88">
+      <c r="I17" s="61">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="L17" s="120">
+      <c r="L17" s="90">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="M17" s="94">
+      <c r="M17" s="67">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="N17" s="95">
+      <c r="N17" s="68">
         <f t="shared" si="4"/>
         <v>36</v>
       </c>
-      <c r="O17" s="95">
+      <c r="O17" s="68">
         <f t="shared" si="5"/>
         <v>46</v>
       </c>
-      <c r="P17" s="96">
+      <c r="P17" s="69">
         <f t="shared" si="6"/>
         <v>56</v>
       </c>
     </row>
     <row r="18" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C18" s="85">
+      <c r="C18" s="58">
         <f t="shared" si="7"/>
         <v>24</v>
       </c>
-      <c r="D18" s="86">
+      <c r="D18" s="59">
         <f t="shared" si="7"/>
         <v>9</v>
       </c>
-      <c r="E18" s="87">
+      <c r="E18" s="60">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="F18" s="87">
+      <c r="F18" s="60">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="G18" s="87">
+      <c r="G18" s="60">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="H18" s="87">
+      <c r="H18" s="60">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I18" s="88">
+      <c r="I18" s="61">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="L18" s="120">
+      <c r="L18" s="90">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="M18" s="94">
+      <c r="M18" s="67">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="N18" s="95">
+      <c r="N18" s="68">
         <f t="shared" si="4"/>
         <v>38</v>
       </c>
-      <c r="O18" s="95">
+      <c r="O18" s="68">
         <f t="shared" si="5"/>
         <v>48</v>
       </c>
-      <c r="P18" s="96">
+      <c r="P18" s="69">
         <f t="shared" si="6"/>
         <v>58</v>
       </c>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C19" s="85">
+      <c r="C19" s="58">
         <f t="shared" si="7"/>
         <v>25</v>
       </c>
-      <c r="D19" s="86">
+      <c r="D19" s="59">
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
-      <c r="E19" s="87">
+      <c r="E19" s="60">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="F19" s="87">
+      <c r="F19" s="60">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="G19" s="87">
+      <c r="G19" s="60">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="H19" s="87">
+      <c r="H19" s="60">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="I19" s="88">
+      <c r="I19" s="61">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="L19" s="120">
+      <c r="L19" s="90">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="M19" s="94">
+      <c r="M19" s="67">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="N19" s="95">
+      <c r="N19" s="68">
         <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="O19" s="95">
+      <c r="O19" s="68">
         <f t="shared" si="5"/>
         <v>50</v>
       </c>
-      <c r="P19" s="96">
+      <c r="P19" s="69">
         <f t="shared" si="6"/>
         <v>60</v>
       </c>
     </row>
     <row r="20" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C20" s="85">
+      <c r="C20" s="58">
         <f t="shared" si="7"/>
         <v>26</v>
       </c>
-      <c r="D20" s="86">
+      <c r="D20" s="59">
         <f t="shared" si="7"/>
         <v>11</v>
       </c>
-      <c r="E20" s="87">
+      <c r="E20" s="60">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="F20" s="87">
+      <c r="F20" s="60">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="G20" s="87">
+      <c r="G20" s="60">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="H20" s="87">
+      <c r="H20" s="60">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="I20" s="88">
+      <c r="I20" s="61">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="L20" s="120">
+      <c r="L20" s="90">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="M20" s="94">
+      <c r="M20" s="67">
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="N20" s="95">
+      <c r="N20" s="68">
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="O20" s="95">
+      <c r="O20" s="68">
         <f t="shared" si="5"/>
         <v>52</v>
       </c>
-      <c r="P20" s="96">
+      <c r="P20" s="69">
         <f t="shared" si="6"/>
         <v>62</v>
       </c>
     </row>
     <row r="21" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C21" s="85">
+      <c r="C21" s="58">
         <f t="shared" si="7"/>
         <v>27</v>
       </c>
-      <c r="D21" s="86">
+      <c r="D21" s="59">
         <f t="shared" si="7"/>
         <v>12</v>
       </c>
-      <c r="E21" s="87">
+      <c r="E21" s="60">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="F21" s="87">
+      <c r="F21" s="60">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="G21" s="87">
+      <c r="G21" s="60">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="H21" s="87">
+      <c r="H21" s="60">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="I21" s="88">
+      <c r="I21" s="61">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="L21" s="120">
+      <c r="L21" s="90">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="M21" s="94">
+      <c r="M21" s="67">
         <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="N21" s="95">
+      <c r="N21" s="68">
         <f t="shared" si="4"/>
         <v>44</v>
       </c>
-      <c r="O21" s="95">
+      <c r="O21" s="68">
         <f t="shared" si="5"/>
         <v>54</v>
       </c>
-      <c r="P21" s="96">
+      <c r="P21" s="69">
         <f t="shared" si="6"/>
         <v>64</v>
       </c>
     </row>
     <row r="22" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C22" s="85">
+      <c r="C22" s="58">
         <f t="shared" si="7"/>
         <v>28</v>
       </c>
-      <c r="D22" s="86">
+      <c r="D22" s="59">
         <f t="shared" si="7"/>
         <v>13</v>
       </c>
-      <c r="E22" s="87">
+      <c r="E22" s="60">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="F22" s="87">
+      <c r="F22" s="60">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="G22" s="87">
+      <c r="G22" s="60">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="H22" s="87">
+      <c r="H22" s="60">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="I22" s="88">
+      <c r="I22" s="61">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="L22" s="120">
+      <c r="L22" s="90">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="M22" s="94">
+      <c r="M22" s="67">
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="N22" s="95">
+      <c r="N22" s="68">
         <f t="shared" si="4"/>
         <v>46</v>
       </c>
-      <c r="O22" s="95">
+      <c r="O22" s="68">
         <f t="shared" si="5"/>
         <v>56</v>
       </c>
-      <c r="P22" s="96">
+      <c r="P22" s="69">
         <f t="shared" si="6"/>
         <v>66</v>
       </c>
     </row>
     <row r="23" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C23" s="85">
+      <c r="C23" s="58">
         <f t="shared" si="7"/>
         <v>29</v>
       </c>
-      <c r="D23" s="86">
+      <c r="D23" s="59">
         <f t="shared" si="7"/>
         <v>14</v>
       </c>
-      <c r="E23" s="87">
+      <c r="E23" s="60">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="F23" s="87">
+      <c r="F23" s="60">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="G23" s="87">
+      <c r="G23" s="60">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="H23" s="87">
+      <c r="H23" s="60">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="I23" s="88">
+      <c r="I23" s="61">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="L23" s="120">
+      <c r="L23" s="90">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="M23" s="94">
+      <c r="M23" s="67">
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
-      <c r="N23" s="95">
+      <c r="N23" s="68">
         <f t="shared" si="4"/>
         <v>48</v>
       </c>
-      <c r="O23" s="95">
+      <c r="O23" s="68">
         <f t="shared" si="5"/>
         <v>58</v>
       </c>
-      <c r="P23" s="96">
+      <c r="P23" s="69">
         <f t="shared" si="6"/>
         <v>68</v>
       </c>
     </row>
     <row r="24" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C24" s="85">
+      <c r="C24" s="58">
         <f t="shared" si="7"/>
         <v>30</v>
       </c>
-      <c r="D24" s="86">
+      <c r="D24" s="59">
         <f t="shared" si="7"/>
         <v>15</v>
       </c>
-      <c r="E24" s="87">
+      <c r="E24" s="60">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="F24" s="87">
+      <c r="F24" s="60">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="G24" s="87">
+      <c r="G24" s="60">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="H24" s="87">
+      <c r="H24" s="60">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="I24" s="88">
+      <c r="I24" s="61">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="L24" s="120">
+      <c r="L24" s="90">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="M24" s="94">
+      <c r="M24" s="67">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="N24" s="95">
+      <c r="N24" s="68">
         <f t="shared" si="4"/>
         <v>50</v>
       </c>
-      <c r="O24" s="95">
+      <c r="O24" s="68">
         <f t="shared" si="5"/>
         <v>60</v>
       </c>
-      <c r="P24" s="96">
+      <c r="P24" s="69">
         <f t="shared" si="6"/>
         <v>70</v>
       </c>
     </row>
     <row r="25" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C25" s="85">
+      <c r="C25" s="58">
         <f t="shared" si="7"/>
         <v>31</v>
       </c>
-      <c r="D25" s="86">
+      <c r="D25" s="59">
         <f t="shared" si="7"/>
         <v>16</v>
       </c>
-      <c r="E25" s="87">
+      <c r="E25" s="60">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="F25" s="87">
+      <c r="F25" s="60">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="G25" s="87">
+      <c r="G25" s="60">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="H25" s="87">
+      <c r="H25" s="60">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="I25" s="88">
+      <c r="I25" s="61">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="L25" s="120">
+      <c r="L25" s="90">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="M25" s="94">
+      <c r="M25" s="67">
         <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="N25" s="95">
+      <c r="N25" s="68">
         <f t="shared" si="4"/>
         <v>52</v>
       </c>
-      <c r="O25" s="95">
+      <c r="O25" s="68">
         <f t="shared" si="5"/>
         <v>62</v>
       </c>
-      <c r="P25" s="96">
+      <c r="P25" s="69">
         <f t="shared" si="6"/>
         <v>72</v>
       </c>
     </row>
     <row r="26" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C26" s="85">
+      <c r="C26" s="58">
         <f t="shared" si="7"/>
         <v>32</v>
       </c>
-      <c r="D26" s="86">
+      <c r="D26" s="59">
         <f t="shared" si="7"/>
         <v>17</v>
       </c>
-      <c r="E26" s="87">
+      <c r="E26" s="60">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="F26" s="87">
+      <c r="F26" s="60">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="G26" s="87">
+      <c r="G26" s="60">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="H26" s="87">
+      <c r="H26" s="60">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="I26" s="88">
+      <c r="I26" s="61">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="L26" s="120">
+      <c r="L26" s="90">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="M26" s="94">
+      <c r="M26" s="67">
         <f t="shared" si="3"/>
         <v>44</v>
       </c>
-      <c r="N26" s="95">
+      <c r="N26" s="68">
         <f t="shared" si="4"/>
         <v>54</v>
       </c>
-      <c r="O26" s="95">
+      <c r="O26" s="68">
         <f t="shared" si="5"/>
         <v>64</v>
       </c>
-      <c r="P26" s="96">
+      <c r="P26" s="69">
         <f t="shared" si="6"/>
         <v>74</v>
       </c>
     </row>
     <row r="27" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C27" s="85">
+      <c r="C27" s="58">
         <f t="shared" si="7"/>
         <v>33</v>
       </c>
-      <c r="D27" s="86">
+      <c r="D27" s="59">
         <f t="shared" si="7"/>
         <v>18</v>
       </c>
-      <c r="E27" s="87">
+      <c r="E27" s="60">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="F27" s="87">
+      <c r="F27" s="60">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="G27" s="87">
+      <c r="G27" s="60">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="H27" s="87">
+      <c r="H27" s="60">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="I27" s="88">
+      <c r="I27" s="61">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="L27" s="120">
+      <c r="L27" s="90">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="M27" s="94">
+      <c r="M27" s="67">
         <f t="shared" si="3"/>
         <v>46</v>
       </c>
-      <c r="N27" s="95">
+      <c r="N27" s="68">
         <f t="shared" si="4"/>
         <v>56</v>
       </c>
-      <c r="O27" s="95">
+      <c r="O27" s="68">
         <f t="shared" si="5"/>
         <v>66</v>
       </c>
-      <c r="P27" s="96">
+      <c r="P27" s="69">
         <f t="shared" si="6"/>
         <v>76</v>
       </c>
     </row>
     <row r="28" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C28" s="85">
+      <c r="C28" s="58">
         <f t="shared" ref="C28:D43" si="8">C27+1</f>
         <v>34</v>
       </c>
-      <c r="D28" s="86">
+      <c r="D28" s="59">
         <f t="shared" si="8"/>
         <v>19</v>
       </c>
-      <c r="E28" s="87">
+      <c r="E28" s="60">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="F28" s="87">
+      <c r="F28" s="60">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="G28" s="87">
+      <c r="G28" s="60">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="H28" s="87">
+      <c r="H28" s="60">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="I28" s="88">
+      <c r="I28" s="61">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="L28" s="120">
+      <c r="L28" s="90">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="M28" s="94">
+      <c r="M28" s="67">
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="N28" s="95">
+      <c r="N28" s="68">
         <f t="shared" si="4"/>
         <v>58</v>
       </c>
-      <c r="O28" s="95">
+      <c r="O28" s="68">
         <f t="shared" si="5"/>
         <v>68</v>
       </c>
-      <c r="P28" s="96">
+      <c r="P28" s="69">
         <f t="shared" si="6"/>
         <v>78</v>
       </c>
     </row>
     <row r="29" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C29" s="85">
+      <c r="C29" s="58">
         <f t="shared" si="8"/>
         <v>35</v>
       </c>
-      <c r="D29" s="86">
+      <c r="D29" s="59">
         <f t="shared" si="8"/>
         <v>20</v>
       </c>
-      <c r="E29" s="87">
+      <c r="E29" s="60">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="F29" s="87">
+      <c r="F29" s="60">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="G29" s="87">
+      <c r="G29" s="60">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="H29" s="87">
+      <c r="H29" s="60">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="I29" s="88">
+      <c r="I29" s="61">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="L29" s="120">
+      <c r="L29" s="90">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="M29" s="94">
+      <c r="M29" s="67">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="N29" s="95">
+      <c r="N29" s="68">
         <f t="shared" si="4"/>
         <v>60</v>
       </c>
-      <c r="O29" s="95">
+      <c r="O29" s="68">
         <f t="shared" si="5"/>
         <v>70</v>
       </c>
-      <c r="P29" s="96">
+      <c r="P29" s="69">
         <f t="shared" si="6"/>
         <v>80</v>
       </c>
     </row>
     <row r="30" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C30" s="85">
+      <c r="C30" s="58">
         <f t="shared" si="8"/>
         <v>36</v>
       </c>
-      <c r="D30" s="86">
+      <c r="D30" s="59">
         <f t="shared" si="8"/>
         <v>21</v>
       </c>
-      <c r="E30" s="87">
+      <c r="E30" s="60">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="F30" s="87">
+      <c r="F30" s="60">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="G30" s="87">
+      <c r="G30" s="60">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="H30" s="87">
+      <c r="H30" s="60">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="I30" s="88">
+      <c r="I30" s="61">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="L30" s="120">
+      <c r="L30" s="90">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="M30" s="94">
+      <c r="M30" s="67">
         <f t="shared" si="3"/>
         <v>52</v>
       </c>
-      <c r="N30" s="95">
+      <c r="N30" s="68">
         <f t="shared" si="4"/>
         <v>62</v>
       </c>
-      <c r="O30" s="95">
+      <c r="O30" s="68">
         <f t="shared" si="5"/>
         <v>72</v>
       </c>
-      <c r="P30" s="96">
+      <c r="P30" s="69">
         <f t="shared" si="6"/>
         <v>82</v>
       </c>
     </row>
     <row r="31" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C31" s="85">
+      <c r="C31" s="58">
         <f t="shared" si="8"/>
         <v>37</v>
       </c>
-      <c r="D31" s="86">
+      <c r="D31" s="59">
         <f t="shared" si="8"/>
         <v>22</v>
       </c>
-      <c r="E31" s="87">
+      <c r="E31" s="60">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="F31" s="87">
+      <c r="F31" s="60">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="G31" s="87">
+      <c r="G31" s="60">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="H31" s="87">
+      <c r="H31" s="60">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="I31" s="88">
+      <c r="I31" s="61">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="L31" s="120">
+      <c r="L31" s="90">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="M31" s="94">
+      <c r="M31" s="67">
         <f t="shared" si="3"/>
         <v>54</v>
       </c>
-      <c r="N31" s="95">
+      <c r="N31" s="68">
         <f t="shared" si="4"/>
         <v>64</v>
       </c>
-      <c r="O31" s="95">
+      <c r="O31" s="68">
         <f t="shared" si="5"/>
         <v>74</v>
       </c>
-      <c r="P31" s="96">
+      <c r="P31" s="69">
         <f t="shared" si="6"/>
         <v>84</v>
       </c>
     </row>
     <row r="32" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C32" s="85">
+      <c r="C32" s="58">
         <f t="shared" si="8"/>
         <v>38</v>
       </c>
-      <c r="D32" s="86">
+      <c r="D32" s="59">
         <f t="shared" si="8"/>
         <v>23</v>
       </c>
-      <c r="E32" s="87">
+      <c r="E32" s="60">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="F32" s="87">
+      <c r="F32" s="60">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="G32" s="87">
+      <c r="G32" s="60">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="H32" s="87">
+      <c r="H32" s="60">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="I32" s="88">
+      <c r="I32" s="61">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="L32" s="120">
+      <c r="L32" s="90">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="M32" s="94">
+      <c r="M32" s="67">
         <f t="shared" si="3"/>
         <v>56</v>
       </c>
-      <c r="N32" s="95">
+      <c r="N32" s="68">
         <f t="shared" si="4"/>
         <v>66</v>
       </c>
-      <c r="O32" s="95">
+      <c r="O32" s="68">
         <f t="shared" si="5"/>
         <v>76</v>
       </c>
-      <c r="P32" s="96">
+      <c r="P32" s="69">
         <f t="shared" si="6"/>
         <v>86</v>
       </c>
     </row>
     <row r="33" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C33" s="85">
+      <c r="C33" s="58">
         <f t="shared" si="8"/>
         <v>39</v>
       </c>
-      <c r="D33" s="86">
+      <c r="D33" s="59">
         <f t="shared" si="8"/>
         <v>24</v>
       </c>
-      <c r="E33" s="87">
+      <c r="E33" s="60">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="F33" s="87">
+      <c r="F33" s="60">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="G33" s="87">
+      <c r="G33" s="60">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="H33" s="87">
+      <c r="H33" s="60">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="I33" s="88">
+      <c r="I33" s="61">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="L33" s="120">
+      <c r="L33" s="90">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="M33" s="94">
+      <c r="M33" s="67">
         <f t="shared" si="3"/>
         <v>58</v>
       </c>
-      <c r="N33" s="95">
+      <c r="N33" s="68">
         <f t="shared" si="4"/>
         <v>68</v>
       </c>
-      <c r="O33" s="95">
+      <c r="O33" s="68">
         <f t="shared" si="5"/>
         <v>78</v>
       </c>
-      <c r="P33" s="96">
+      <c r="P33" s="69">
         <f t="shared" si="6"/>
         <v>88</v>
       </c>
     </row>
     <row r="34" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C34" s="85">
+      <c r="C34" s="58">
         <f t="shared" si="8"/>
         <v>40</v>
       </c>
-      <c r="D34" s="86">
+      <c r="D34" s="59">
         <f t="shared" si="8"/>
         <v>25</v>
       </c>
-      <c r="E34" s="87">
+      <c r="E34" s="60">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="F34" s="87">
+      <c r="F34" s="60">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="G34" s="87">
+      <c r="G34" s="60">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="H34" s="87">
+      <c r="H34" s="60">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="I34" s="88">
+      <c r="I34" s="61">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="L34" s="120">
+      <c r="L34" s="90">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="M34" s="94">
+      <c r="M34" s="67">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="N34" s="95">
+      <c r="N34" s="68">
         <f t="shared" si="4"/>
         <v>70</v>
       </c>
-      <c r="O34" s="95">
+      <c r="O34" s="68">
         <f t="shared" si="5"/>
         <v>80</v>
       </c>
-      <c r="P34" s="96">
+      <c r="P34" s="69">
         <f t="shared" si="6"/>
         <v>90</v>
       </c>
     </row>
     <row r="35" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C35" s="85">
+      <c r="C35" s="58">
         <f t="shared" si="8"/>
         <v>41</v>
       </c>
-      <c r="D35" s="86">
+      <c r="D35" s="59">
         <f t="shared" si="8"/>
         <v>26</v>
       </c>
-      <c r="E35" s="87">
+      <c r="E35" s="60">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="F35" s="87">
+      <c r="F35" s="60">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="G35" s="87">
+      <c r="G35" s="60">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="H35" s="87">
+      <c r="H35" s="60">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="I35" s="88">
+      <c r="I35" s="61">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="L35" s="120">
+      <c r="L35" s="90">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="M35" s="94">
+      <c r="M35" s="67">
         <f t="shared" si="3"/>
         <v>62</v>
       </c>
-      <c r="N35" s="95">
+      <c r="N35" s="68">
         <f t="shared" si="4"/>
         <v>72</v>
       </c>
-      <c r="O35" s="95">
+      <c r="O35" s="68">
         <f t="shared" si="5"/>
         <v>82</v>
       </c>
-      <c r="P35" s="96">
+      <c r="P35" s="69">
         <f t="shared" si="6"/>
         <v>92</v>
       </c>
     </row>
     <row r="36" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C36" s="85">
+      <c r="C36" s="58">
         <f t="shared" si="8"/>
         <v>42</v>
       </c>
-      <c r="D36" s="86">
+      <c r="D36" s="59">
         <f t="shared" si="8"/>
         <v>27</v>
       </c>
-      <c r="E36" s="87">
+      <c r="E36" s="60">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="F36" s="87">
+      <c r="F36" s="60">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="G36" s="87">
+      <c r="G36" s="60">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="H36" s="87">
+      <c r="H36" s="60">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="I36" s="88">
+      <c r="I36" s="61">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="L36" s="120">
+      <c r="L36" s="90">
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="M36" s="94">
+      <c r="M36" s="67">
         <f t="shared" si="3"/>
         <v>64</v>
       </c>
-      <c r="N36" s="95">
+      <c r="N36" s="68">
         <f t="shared" si="4"/>
         <v>74</v>
       </c>
-      <c r="O36" s="95">
+      <c r="O36" s="68">
         <f t="shared" si="5"/>
         <v>84</v>
       </c>
-      <c r="P36" s="96">
+      <c r="P36" s="69">
         <f t="shared" si="6"/>
         <v>94</v>
       </c>
     </row>
     <row r="37" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C37" s="85">
+      <c r="C37" s="58">
         <f t="shared" si="8"/>
         <v>43</v>
       </c>
-      <c r="D37" s="86">
+      <c r="D37" s="59">
         <f t="shared" si="8"/>
         <v>28</v>
       </c>
-      <c r="E37" s="87">
+      <c r="E37" s="60">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="F37" s="87">
+      <c r="F37" s="60">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="G37" s="87">
+      <c r="G37" s="60">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="H37" s="87">
+      <c r="H37" s="60">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="I37" s="88">
+      <c r="I37" s="61">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="L37" s="120">
+      <c r="L37" s="90">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="M37" s="94">
+      <c r="M37" s="67">
         <f t="shared" si="3"/>
         <v>66</v>
       </c>
-      <c r="N37" s="95">
+      <c r="N37" s="68">
         <f t="shared" si="4"/>
         <v>76</v>
       </c>
-      <c r="O37" s="95">
+      <c r="O37" s="68">
         <f t="shared" si="5"/>
         <v>86</v>
       </c>
-      <c r="P37" s="96">
+      <c r="P37" s="69">
         <f t="shared" si="6"/>
         <v>96</v>
       </c>
     </row>
     <row r="38" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C38" s="85">
+      <c r="C38" s="58">
         <f t="shared" si="8"/>
         <v>44</v>
       </c>
-      <c r="D38" s="86">
+      <c r="D38" s="59">
         <f t="shared" si="8"/>
         <v>29</v>
       </c>
-      <c r="E38" s="87">
+      <c r="E38" s="60">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="F38" s="87">
+      <c r="F38" s="60">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="G38" s="87">
+      <c r="G38" s="60">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="H38" s="87">
+      <c r="H38" s="60">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="I38" s="88">
+      <c r="I38" s="61">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="L38" s="120">
+      <c r="L38" s="90">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="M38" s="94">
+      <c r="M38" s="67">
         <f t="shared" si="3"/>
         <v>68</v>
       </c>
-      <c r="N38" s="95">
+      <c r="N38" s="68">
         <f t="shared" si="4"/>
         <v>78</v>
       </c>
-      <c r="O38" s="95">
+      <c r="O38" s="68">
         <f t="shared" si="5"/>
         <v>88</v>
       </c>
-      <c r="P38" s="96">
+      <c r="P38" s="69">
         <f t="shared" si="6"/>
         <v>98</v>
       </c>
     </row>
     <row r="39" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C39" s="85">
+      <c r="C39" s="58">
         <f t="shared" si="8"/>
         <v>45</v>
       </c>
-      <c r="D39" s="86">
+      <c r="D39" s="59">
         <f t="shared" si="8"/>
         <v>30</v>
       </c>
-      <c r="E39" s="87">
+      <c r="E39" s="60">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="F39" s="87">
+      <c r="F39" s="60">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="G39" s="87">
+      <c r="G39" s="60">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="H39" s="87">
+      <c r="H39" s="60">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="I39" s="88">
+      <c r="I39" s="61">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="L39" s="120">
+      <c r="L39" s="90">
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="M39" s="94">
+      <c r="M39" s="67">
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="N39" s="95">
+      <c r="N39" s="68">
         <f t="shared" si="4"/>
         <v>80</v>
       </c>
-      <c r="O39" s="95">
+      <c r="O39" s="68">
         <f t="shared" si="5"/>
         <v>90</v>
       </c>
-      <c r="P39" s="96">
+      <c r="P39" s="69">
         <f t="shared" si="6"/>
         <v>100</v>
       </c>
     </row>
     <row r="40" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C40" s="85">
+      <c r="C40" s="58">
         <f t="shared" si="8"/>
         <v>46</v>
       </c>
-      <c r="D40" s="86">
+      <c r="D40" s="59">
         <f t="shared" si="8"/>
         <v>31</v>
       </c>
-      <c r="E40" s="87">
+      <c r="E40" s="60">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="F40" s="87">
+      <c r="F40" s="60">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="G40" s="87">
+      <c r="G40" s="60">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="H40" s="87">
+      <c r="H40" s="60">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="I40" s="88">
+      <c r="I40" s="61">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="L40" s="120">
+      <c r="L40" s="90">
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="M40" s="94">
+      <c r="M40" s="67">
         <f t="shared" si="3"/>
         <v>72</v>
       </c>
-      <c r="N40" s="95">
+      <c r="N40" s="68">
         <f t="shared" si="4"/>
         <v>82</v>
       </c>
-      <c r="O40" s="95">
+      <c r="O40" s="68">
         <f t="shared" si="5"/>
         <v>92</v>
       </c>
-      <c r="P40" s="96">
+      <c r="P40" s="69">
         <f t="shared" si="6"/>
         <v>102</v>
       </c>
     </row>
     <row r="41" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C41" s="85">
+      <c r="C41" s="58">
         <f t="shared" si="8"/>
         <v>47</v>
       </c>
-      <c r="D41" s="86">
+      <c r="D41" s="59">
         <f t="shared" si="8"/>
         <v>32</v>
       </c>
-      <c r="E41" s="87">
+      <c r="E41" s="60">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="F41" s="87">
+      <c r="F41" s="60">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="G41" s="87">
+      <c r="G41" s="60">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="H41" s="87">
+      <c r="H41" s="60">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="I41" s="88">
+      <c r="I41" s="61">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="L41" s="120">
+      <c r="L41" s="90">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="M41" s="94">
+      <c r="M41" s="67">
         <f t="shared" si="3"/>
         <v>74</v>
       </c>
-      <c r="N41" s="95">
+      <c r="N41" s="68">
         <f t="shared" si="4"/>
         <v>84</v>
       </c>
-      <c r="O41" s="95">
+      <c r="O41" s="68">
         <f t="shared" si="5"/>
         <v>94</v>
       </c>
-      <c r="P41" s="96">
+      <c r="P41" s="69">
         <f t="shared" si="6"/>
         <v>104</v>
       </c>
     </row>
     <row r="42" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C42" s="85">
+      <c r="C42" s="58">
         <f t="shared" si="8"/>
         <v>48</v>
       </c>
-      <c r="D42" s="86">
+      <c r="D42" s="59">
         <f t="shared" si="8"/>
         <v>33</v>
       </c>
-      <c r="E42" s="87">
+      <c r="E42" s="60">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="F42" s="87">
+      <c r="F42" s="60">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="G42" s="87">
+      <c r="G42" s="60">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="H42" s="87">
+      <c r="H42" s="60">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="I42" s="88">
+      <c r="I42" s="61">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="L42" s="120">
+      <c r="L42" s="90">
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="M42" s="94">
+      <c r="M42" s="67">
         <f t="shared" si="3"/>
         <v>76</v>
       </c>
-      <c r="N42" s="95">
+      <c r="N42" s="68">
         <f t="shared" si="4"/>
         <v>86</v>
       </c>
-      <c r="O42" s="95">
+      <c r="O42" s="68">
         <f t="shared" si="5"/>
         <v>96</v>
       </c>
-      <c r="P42" s="96">
+      <c r="P42" s="69">
         <f t="shared" si="6"/>
         <v>106</v>
       </c>
     </row>
     <row r="43" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C43" s="85">
+      <c r="C43" s="58">
         <f t="shared" si="8"/>
         <v>49</v>
       </c>
-      <c r="D43" s="86">
+      <c r="D43" s="59">
         <f t="shared" si="8"/>
         <v>34</v>
       </c>
-      <c r="E43" s="87">
+      <c r="E43" s="60">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="F43" s="87">
+      <c r="F43" s="60">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="G43" s="87">
+      <c r="G43" s="60">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="H43" s="87">
+      <c r="H43" s="60">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="I43" s="88">
+      <c r="I43" s="61">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="L43" s="120">
+      <c r="L43" s="90">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="M43" s="94">
+      <c r="M43" s="67">
         <f t="shared" si="3"/>
         <v>78</v>
       </c>
-      <c r="N43" s="95">
+      <c r="N43" s="68">
         <f t="shared" si="4"/>
         <v>88</v>
       </c>
-      <c r="O43" s="95">
+      <c r="O43" s="68">
         <f t="shared" si="5"/>
         <v>98</v>
       </c>
-      <c r="P43" s="96">
+      <c r="P43" s="69">
         <f t="shared" si="6"/>
         <v>108</v>
       </c>
     </row>
     <row r="44" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C44" s="85">
+      <c r="C44" s="58">
         <f t="shared" ref="C44:D59" si="9">C43+1</f>
         <v>50</v>
       </c>
-      <c r="D44" s="86">
+      <c r="D44" s="59">
         <f t="shared" si="9"/>
         <v>35</v>
       </c>
-      <c r="E44" s="87">
+      <c r="E44" s="60">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="F44" s="87">
+      <c r="F44" s="60">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="G44" s="87">
+      <c r="G44" s="60">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="H44" s="87">
+      <c r="H44" s="60">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="I44" s="88">
+      <c r="I44" s="61">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="L44" s="120">
+      <c r="L44" s="90">
         <f t="shared" si="2"/>
         <v>51</v>
       </c>
-      <c r="M44" s="94">
+      <c r="M44" s="67">
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="N44" s="95">
+      <c r="N44" s="68">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
-      <c r="O44" s="95">
+      <c r="O44" s="68">
         <f t="shared" si="5"/>
         <v>100</v>
       </c>
-      <c r="P44" s="96">
+      <c r="P44" s="69">
         <f t="shared" si="6"/>
         <v>110</v>
       </c>
     </row>
     <row r="45" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C45" s="85">
+      <c r="C45" s="58">
         <f t="shared" si="9"/>
         <v>51</v>
       </c>
-      <c r="D45" s="86">
+      <c r="D45" s="59">
         <f t="shared" si="9"/>
         <v>36</v>
       </c>
-      <c r="E45" s="87">
+      <c r="E45" s="60">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="F45" s="87">
+      <c r="F45" s="60">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="G45" s="87">
+      <c r="G45" s="60">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="H45" s="87">
+      <c r="H45" s="60">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="I45" s="88">
+      <c r="I45" s="61">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="L45" s="120">
+      <c r="L45" s="90">
         <f t="shared" si="2"/>
         <v>52</v>
       </c>
-      <c r="M45" s="94">
+      <c r="M45" s="67">
         <f t="shared" si="3"/>
         <v>82</v>
       </c>
-      <c r="N45" s="95">
+      <c r="N45" s="68">
         <f t="shared" si="4"/>
         <v>92</v>
       </c>
-      <c r="O45" s="95">
+      <c r="O45" s="68">
         <f t="shared" si="5"/>
         <v>102</v>
       </c>
-      <c r="P45" s="96">
+      <c r="P45" s="69">
         <f t="shared" si="6"/>
         <v>112</v>
       </c>
     </row>
     <row r="46" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C46" s="85">
+      <c r="C46" s="58">
         <f t="shared" si="9"/>
         <v>52</v>
       </c>
-      <c r="D46" s="86">
+      <c r="D46" s="59">
         <f t="shared" si="9"/>
         <v>37</v>
       </c>
-      <c r="E46" s="87">
+      <c r="E46" s="60">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="F46" s="87">
+      <c r="F46" s="60">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="G46" s="87">
+      <c r="G46" s="60">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="H46" s="87">
+      <c r="H46" s="60">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="I46" s="88">
+      <c r="I46" s="61">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="L46" s="120">
+      <c r="L46" s="90">
         <f t="shared" si="2"/>
         <v>53</v>
       </c>
-      <c r="M46" s="94">
+      <c r="M46" s="67">
         <f t="shared" si="3"/>
         <v>84</v>
       </c>
-      <c r="N46" s="95">
+      <c r="N46" s="68">
         <f t="shared" si="4"/>
         <v>94</v>
       </c>
-      <c r="O46" s="95">
+      <c r="O46" s="68">
         <f t="shared" si="5"/>
         <v>104</v>
       </c>
-      <c r="P46" s="96">
+      <c r="P46" s="69">
         <f t="shared" si="6"/>
         <v>114</v>
       </c>
     </row>
     <row r="47" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C47" s="85">
+      <c r="C47" s="58">
         <f t="shared" si="9"/>
         <v>53</v>
       </c>
-      <c r="D47" s="86">
+      <c r="D47" s="59">
         <f t="shared" si="9"/>
         <v>38</v>
       </c>
-      <c r="E47" s="87">
+      <c r="E47" s="60">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="F47" s="87">
+      <c r="F47" s="60">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="G47" s="87">
+      <c r="G47" s="60">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="H47" s="87">
+      <c r="H47" s="60">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="I47" s="88">
+      <c r="I47" s="61">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="L47" s="120">
+      <c r="L47" s="90">
         <f t="shared" si="2"/>
         <v>54</v>
       </c>
-      <c r="M47" s="94">
+      <c r="M47" s="67">
         <f t="shared" si="3"/>
         <v>86</v>
       </c>
-      <c r="N47" s="95">
+      <c r="N47" s="68">
         <f t="shared" si="4"/>
         <v>96</v>
       </c>
-      <c r="O47" s="95">
+      <c r="O47" s="68">
         <f t="shared" si="5"/>
         <v>106</v>
       </c>
-      <c r="P47" s="96">
+      <c r="P47" s="69">
         <f t="shared" si="6"/>
         <v>116</v>
       </c>
     </row>
     <row r="48" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C48" s="85">
+      <c r="C48" s="58">
         <f t="shared" si="9"/>
         <v>54</v>
       </c>
-      <c r="D48" s="86">
+      <c r="D48" s="59">
         <f t="shared" si="9"/>
         <v>39</v>
       </c>
-      <c r="E48" s="87">
+      <c r="E48" s="60">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="F48" s="87">
+      <c r="F48" s="60">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="G48" s="87">
+      <c r="G48" s="60">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="H48" s="87">
+      <c r="H48" s="60">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="I48" s="88">
+      <c r="I48" s="61">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="L48" s="120">
+      <c r="L48" s="90">
         <f t="shared" si="2"/>
         <v>55</v>
       </c>
-      <c r="M48" s="94">
+      <c r="M48" s="67">
         <f t="shared" si="3"/>
         <v>88</v>
       </c>
-      <c r="N48" s="95">
+      <c r="N48" s="68">
         <f t="shared" si="4"/>
         <v>98</v>
       </c>
-      <c r="O48" s="95">
+      <c r="O48" s="68">
         <f t="shared" si="5"/>
         <v>108</v>
       </c>
-      <c r="P48" s="96">
+      <c r="P48" s="69">
         <f t="shared" si="6"/>
         <v>118</v>
       </c>
     </row>
     <row r="49" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C49" s="85">
+      <c r="C49" s="58">
         <f t="shared" si="9"/>
         <v>55</v>
       </c>
-      <c r="D49" s="86">
+      <c r="D49" s="59">
         <f t="shared" si="9"/>
         <v>40</v>
       </c>
-      <c r="E49" s="87">
+      <c r="E49" s="60">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="F49" s="87">
+      <c r="F49" s="60">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="G49" s="87">
+      <c r="G49" s="60">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="H49" s="87">
+      <c r="H49" s="60">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="I49" s="88">
+      <c r="I49" s="61">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="L49" s="120">
+      <c r="L49" s="90">
         <f t="shared" si="2"/>
         <v>56</v>
       </c>
-      <c r="M49" s="94">
+      <c r="M49" s="67">
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="N49" s="95">
+      <c r="N49" s="68">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="O49" s="95">
+      <c r="O49" s="68">
         <f t="shared" si="5"/>
         <v>110</v>
       </c>
-      <c r="P49" s="96">
+      <c r="P49" s="69">
         <f t="shared" si="6"/>
         <v>120</v>
       </c>
     </row>
     <row r="50" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C50" s="85">
+      <c r="C50" s="58">
         <f t="shared" si="9"/>
         <v>56</v>
       </c>
-      <c r="D50" s="86">
+      <c r="D50" s="59">
         <f t="shared" si="9"/>
         <v>41</v>
       </c>
-      <c r="E50" s="87">
+      <c r="E50" s="60">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="F50" s="87">
+      <c r="F50" s="60">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="G50" s="87">
+      <c r="G50" s="60">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="H50" s="87">
+      <c r="H50" s="60">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="I50" s="88">
+      <c r="I50" s="61">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="L50" s="120">
+      <c r="L50" s="90">
         <f t="shared" si="2"/>
         <v>57</v>
       </c>
-      <c r="M50" s="94">
+      <c r="M50" s="67">
         <f t="shared" si="3"/>
         <v>92</v>
       </c>
-      <c r="N50" s="95">
+      <c r="N50" s="68">
         <f t="shared" si="4"/>
         <v>102</v>
       </c>
-      <c r="O50" s="95">
+      <c r="O50" s="68">
         <f t="shared" si="5"/>
         <v>112</v>
       </c>
-      <c r="P50" s="96">
+      <c r="P50" s="69">
         <f t="shared" si="6"/>
         <v>122</v>
       </c>
     </row>
     <row r="51" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C51" s="85">
+      <c r="C51" s="58">
         <f t="shared" si="9"/>
         <v>57</v>
       </c>
-      <c r="D51" s="86">
+      <c r="D51" s="59">
         <f t="shared" si="9"/>
         <v>42</v>
       </c>
-      <c r="E51" s="87">
+      <c r="E51" s="60">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="F51" s="87">
+      <c r="F51" s="60">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="G51" s="87">
+      <c r="G51" s="60">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="H51" s="87">
+      <c r="H51" s="60">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="I51" s="88">
+      <c r="I51" s="61">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="L51" s="120">
+      <c r="L51" s="90">
         <f t="shared" si="2"/>
         <v>58</v>
       </c>
-      <c r="M51" s="94">
+      <c r="M51" s="67">
         <f t="shared" si="3"/>
         <v>94</v>
       </c>
-      <c r="N51" s="95">
+      <c r="N51" s="68">
         <f t="shared" si="4"/>
         <v>104</v>
       </c>
-      <c r="O51" s="95">
+      <c r="O51" s="68">
         <f t="shared" si="5"/>
         <v>114</v>
       </c>
-      <c r="P51" s="96">
+      <c r="P51" s="69">
         <f t="shared" si="6"/>
         <v>124</v>
       </c>
     </row>
     <row r="52" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C52" s="85">
+      <c r="C52" s="58">
         <f t="shared" si="9"/>
         <v>58</v>
       </c>
-      <c r="D52" s="86">
+      <c r="D52" s="59">
         <f t="shared" si="9"/>
         <v>43</v>
       </c>
-      <c r="E52" s="87">
+      <c r="E52" s="60">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="F52" s="87">
+      <c r="F52" s="60">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="G52" s="87">
+      <c r="G52" s="60">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="H52" s="87">
+      <c r="H52" s="60">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="I52" s="88">
+      <c r="I52" s="61">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="L52" s="120">
+      <c r="L52" s="90">
         <f t="shared" si="2"/>
         <v>59</v>
       </c>
-      <c r="M52" s="94">
+      <c r="M52" s="67">
         <f t="shared" si="3"/>
         <v>96</v>
       </c>
-      <c r="N52" s="95">
+      <c r="N52" s="68">
         <f t="shared" si="4"/>
         <v>106</v>
       </c>
-      <c r="O52" s="95">
+      <c r="O52" s="68">
         <f t="shared" si="5"/>
         <v>116</v>
       </c>
-      <c r="P52" s="96">
+      <c r="P52" s="69">
         <f t="shared" si="6"/>
         <v>126</v>
       </c>
     </row>
     <row r="53" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C53" s="85">
+      <c r="C53" s="58">
         <f t="shared" si="9"/>
         <v>59</v>
       </c>
-      <c r="D53" s="86">
+      <c r="D53" s="59">
         <f t="shared" si="9"/>
         <v>44</v>
       </c>
-      <c r="E53" s="87">
+      <c r="E53" s="60">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="F53" s="87">
+      <c r="F53" s="60">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="G53" s="87">
+      <c r="G53" s="60">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="H53" s="87">
+      <c r="H53" s="60">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="I53" s="88">
+      <c r="I53" s="61">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="L53" s="120">
+      <c r="L53" s="90">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="M53" s="94">
+      <c r="M53" s="67">
         <f t="shared" si="3"/>
         <v>98</v>
       </c>
-      <c r="N53" s="95">
+      <c r="N53" s="68">
         <f t="shared" si="4"/>
         <v>108</v>
       </c>
-      <c r="O53" s="95">
+      <c r="O53" s="68">
         <f t="shared" si="5"/>
         <v>118</v>
       </c>
-      <c r="P53" s="96">
+      <c r="P53" s="69">
         <f t="shared" si="6"/>
         <v>128</v>
       </c>
     </row>
     <row r="54" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C54" s="85">
+      <c r="C54" s="58">
         <f t="shared" si="9"/>
         <v>60</v>
       </c>
-      <c r="D54" s="86">
+      <c r="D54" s="59">
         <f t="shared" si="9"/>
         <v>45</v>
       </c>
-      <c r="E54" s="87">
+      <c r="E54" s="60">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="F54" s="87">
+      <c r="F54" s="60">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="G54" s="87">
+      <c r="G54" s="60">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="H54" s="87">
+      <c r="H54" s="60">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="I54" s="88">
+      <c r="I54" s="61">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="L54" s="120">
+      <c r="L54" s="90">
         <f t="shared" si="2"/>
         <v>61</v>
       </c>
-      <c r="M54" s="94">
+      <c r="M54" s="67">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="N54" s="95">
+      <c r="N54" s="68">
         <f t="shared" si="4"/>
         <v>110</v>
       </c>
-      <c r="O54" s="95">
+      <c r="O54" s="68">
         <f t="shared" si="5"/>
         <v>120</v>
       </c>
-      <c r="P54" s="96">
+      <c r="P54" s="69">
         <f t="shared" si="6"/>
         <v>130</v>
       </c>
     </row>
     <row r="55" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C55" s="85">
+      <c r="C55" s="58">
         <f t="shared" si="9"/>
         <v>61</v>
       </c>
-      <c r="D55" s="86">
+      <c r="D55" s="59">
         <f t="shared" si="9"/>
         <v>46</v>
       </c>
-      <c r="E55" s="87">
+      <c r="E55" s="60">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="F55" s="87">
+      <c r="F55" s="60">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="G55" s="87">
+      <c r="G55" s="60">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="H55" s="87">
+      <c r="H55" s="60">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="I55" s="88">
+      <c r="I55" s="61">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="L55" s="120">
+      <c r="L55" s="90">
         <f t="shared" si="2"/>
         <v>62</v>
       </c>
-      <c r="M55" s="94">
+      <c r="M55" s="67">
         <f t="shared" si="3"/>
         <v>102</v>
       </c>
-      <c r="N55" s="95">
+      <c r="N55" s="68">
         <f t="shared" si="4"/>
         <v>112</v>
       </c>
-      <c r="O55" s="95">
+      <c r="O55" s="68">
         <f t="shared" si="5"/>
         <v>122</v>
       </c>
-      <c r="P55" s="96">
+      <c r="P55" s="69">
         <f t="shared" si="6"/>
         <v>132</v>
       </c>
     </row>
     <row r="56" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C56" s="85">
+      <c r="C56" s="58">
         <f t="shared" si="9"/>
         <v>62</v>
       </c>
-      <c r="D56" s="86">
+      <c r="D56" s="59">
         <f t="shared" si="9"/>
         <v>47</v>
       </c>
-      <c r="E56" s="87">
+      <c r="E56" s="60">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="F56" s="87">
+      <c r="F56" s="60">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="G56" s="87">
+      <c r="G56" s="60">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="H56" s="87">
+      <c r="H56" s="60">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="I56" s="88">
+      <c r="I56" s="61">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="L56" s="120">
+      <c r="L56" s="90">
         <f t="shared" si="2"/>
         <v>63</v>
       </c>
-      <c r="M56" s="94">
+      <c r="M56" s="67">
         <f t="shared" si="3"/>
         <v>104</v>
       </c>
-      <c r="N56" s="95">
+      <c r="N56" s="68">
         <f t="shared" si="4"/>
         <v>114</v>
       </c>
-      <c r="O56" s="95">
+      <c r="O56" s="68">
         <f t="shared" si="5"/>
         <v>124</v>
       </c>
-      <c r="P56" s="96">
+      <c r="P56" s="69">
         <f t="shared" si="6"/>
         <v>134</v>
       </c>
     </row>
     <row r="57" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C57" s="85">
+      <c r="C57" s="58">
         <f t="shared" si="9"/>
         <v>63</v>
       </c>
-      <c r="D57" s="86">
+      <c r="D57" s="59">
         <f t="shared" si="9"/>
         <v>48</v>
       </c>
-      <c r="E57" s="87">
+      <c r="E57" s="60">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="F57" s="87">
+      <c r="F57" s="60">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="G57" s="87">
+      <c r="G57" s="60">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="H57" s="87">
+      <c r="H57" s="60">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="I57" s="88">
+      <c r="I57" s="61">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="L57" s="120">
+      <c r="L57" s="90">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="M57" s="94">
+      <c r="M57" s="67">
         <f t="shared" si="3"/>
         <v>106</v>
       </c>
-      <c r="N57" s="95">
+      <c r="N57" s="68">
         <f t="shared" si="4"/>
         <v>116</v>
       </c>
-      <c r="O57" s="95">
+      <c r="O57" s="68">
         <f t="shared" si="5"/>
         <v>126</v>
       </c>
-      <c r="P57" s="96">
+      <c r="P57" s="69">
         <f t="shared" si="6"/>
         <v>136</v>
       </c>
     </row>
     <row r="58" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C58" s="85">
+      <c r="C58" s="58">
         <f t="shared" si="9"/>
         <v>64</v>
       </c>
-      <c r="D58" s="86">
+      <c r="D58" s="59">
         <f t="shared" si="9"/>
         <v>49</v>
       </c>
-      <c r="E58" s="87">
+      <c r="E58" s="60">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="F58" s="87">
+      <c r="F58" s="60">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="G58" s="87">
+      <c r="G58" s="60">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="H58" s="87">
+      <c r="H58" s="60">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="I58" s="88">
+      <c r="I58" s="61">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="L58" s="121">
+      <c r="L58" s="91">
         <f t="shared" si="2"/>
         <v>65</v>
       </c>
-      <c r="M58" s="99">
+      <c r="M58" s="72">
         <f t="shared" si="3"/>
         <v>108</v>
       </c>
-      <c r="N58" s="97">
+      <c r="N58" s="70">
         <f t="shared" si="4"/>
         <v>118</v>
       </c>
-      <c r="O58" s="97">
+      <c r="O58" s="70">
         <f t="shared" si="5"/>
         <v>128</v>
       </c>
-      <c r="P58" s="98">
+      <c r="P58" s="71">
         <f t="shared" si="6"/>
         <v>138</v>
       </c>
     </row>
     <row r="59" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C59" s="89">
+      <c r="C59" s="62">
         <f t="shared" si="9"/>
         <v>65</v>
       </c>
-      <c r="D59" s="90">
+      <c r="D59" s="63">
         <f t="shared" si="9"/>
         <v>50</v>
       </c>
-      <c r="E59" s="91">
+      <c r="E59" s="64">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="F59" s="91">
+      <c r="F59" s="64">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="G59" s="91">
+      <c r="G59" s="64">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="H59" s="91">
+      <c r="H59" s="64">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="I59" s="92">
+      <c r="I59" s="65">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
started to refactor to make more testable
</commit_message>
<xml_diff>
--- a/src/main/resources/workbooks/Testing.xlsx
+++ b/src/main/resources/workbooks/Testing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="76">
   <si>
     <t>Policy Number</t>
   </si>
@@ -237,6 +237,27 @@
   </si>
   <si>
     <t>Policy Period Year</t>
+  </si>
+  <si>
+    <t>BC:13</t>
+  </si>
+  <si>
+    <t>BCD:14-15</t>
+  </si>
+  <si>
+    <t>D:13</t>
+  </si>
+  <si>
+    <t>F:13-15</t>
+  </si>
+  <si>
+    <t>E:13</t>
+  </si>
+  <si>
+    <t>E:14</t>
+  </si>
+  <si>
+    <t>E:15</t>
   </si>
 </sst>
 </file>
@@ -768,7 +789,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -991,6 +1012,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1026,6 +1054,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1360,8 +1394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1378,256 +1412,256 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="93"/>
-      <c r="M2" s="93"/>
-      <c r="N2" s="93"/>
-      <c r="O2" s="93"/>
-      <c r="P2" s="93"/>
-      <c r="Q2" s="93"/>
-      <c r="R2" s="93"/>
-      <c r="S2" s="93"/>
-      <c r="T2" s="93"/>
-      <c r="U2" s="93"/>
-      <c r="V2" s="93"/>
-      <c r="W2" s="93"/>
-      <c r="X2" s="93"/>
-      <c r="Y2" s="93"/>
-      <c r="Z2" s="94"/>
-      <c r="AA2" s="92" t="s">
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
+      <c r="Q2" s="96"/>
+      <c r="R2" s="96"/>
+      <c r="S2" s="96"/>
+      <c r="T2" s="96"/>
+      <c r="U2" s="96"/>
+      <c r="V2" s="96"/>
+      <c r="W2" s="96"/>
+      <c r="X2" s="96"/>
+      <c r="Y2" s="96"/>
+      <c r="Z2" s="97"/>
+      <c r="AA2" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="93"/>
-      <c r="AC2" s="93"/>
-      <c r="AD2" s="93"/>
-      <c r="AE2" s="93"/>
-      <c r="AF2" s="93"/>
-      <c r="AG2" s="93"/>
-      <c r="AH2" s="93"/>
-      <c r="AI2" s="93"/>
-      <c r="AJ2" s="93"/>
-      <c r="AK2" s="93"/>
-      <c r="AL2" s="94"/>
+      <c r="AB2" s="96"/>
+      <c r="AC2" s="96"/>
+      <c r="AD2" s="96"/>
+      <c r="AE2" s="96"/>
+      <c r="AF2" s="96"/>
+      <c r="AG2" s="96"/>
+      <c r="AH2" s="96"/>
+      <c r="AI2" s="96"/>
+      <c r="AJ2" s="96"/>
+      <c r="AK2" s="96"/>
+      <c r="AL2" s="97"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="95">
+      <c r="B3" s="98">
         <v>1</v>
       </c>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
-      <c r="N3" s="95"/>
-      <c r="O3" s="95"/>
-      <c r="P3" s="95"/>
-      <c r="Q3" s="95"/>
-      <c r="R3" s="95"/>
-      <c r="S3" s="95"/>
-      <c r="T3" s="95"/>
-      <c r="U3" s="95"/>
-      <c r="V3" s="95"/>
-      <c r="W3" s="95"/>
-      <c r="X3" s="95"/>
-      <c r="Y3" s="95"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
+      <c r="Q3" s="98"/>
+      <c r="R3" s="98"/>
+      <c r="S3" s="98"/>
+      <c r="T3" s="98"/>
+      <c r="U3" s="98"/>
+      <c r="V3" s="98"/>
+      <c r="W3" s="98"/>
+      <c r="X3" s="98"/>
+      <c r="Y3" s="98"/>
       <c r="Z3" s="2">
         <v>2</v>
       </c>
       <c r="AA3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AB3" s="92" t="s">
+      <c r="AB3" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="AC3" s="93"/>
-      <c r="AD3" s="93"/>
-      <c r="AE3" s="93"/>
-      <c r="AF3" s="93"/>
-      <c r="AG3" s="93"/>
-      <c r="AH3" s="93"/>
-      <c r="AI3" s="93"/>
-      <c r="AJ3" s="93"/>
-      <c r="AK3" s="93"/>
-      <c r="AL3" s="94"/>
+      <c r="AC3" s="96"/>
+      <c r="AD3" s="96"/>
+      <c r="AE3" s="96"/>
+      <c r="AF3" s="96"/>
+      <c r="AG3" s="96"/>
+      <c r="AH3" s="96"/>
+      <c r="AI3" s="96"/>
+      <c r="AJ3" s="96"/>
+      <c r="AK3" s="96"/>
+      <c r="AL3" s="97"/>
     </row>
     <row r="4" spans="1:38" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96" t="s">
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96" t="s">
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="96"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96" t="s">
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="96"/>
-      <c r="M4" s="96"/>
-      <c r="N4" s="96" t="s">
+      <c r="L4" s="99"/>
+      <c r="M4" s="99"/>
+      <c r="N4" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="96"/>
-      <c r="P4" s="96"/>
-      <c r="Q4" s="96" t="s">
+      <c r="O4" s="99"/>
+      <c r="P4" s="99"/>
+      <c r="Q4" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="R4" s="96"/>
-      <c r="S4" s="96"/>
-      <c r="T4" s="96" t="s">
+      <c r="R4" s="99"/>
+      <c r="S4" s="99"/>
+      <c r="T4" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="U4" s="96"/>
-      <c r="V4" s="96"/>
-      <c r="W4" s="97" t="s">
+      <c r="U4" s="99"/>
+      <c r="V4" s="99"/>
+      <c r="W4" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="X4" s="98"/>
-      <c r="Y4" s="99"/>
+      <c r="X4" s="101"/>
+      <c r="Y4" s="102"/>
       <c r="Z4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="AA4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="97" t="s">
+      <c r="AB4" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="AC4" s="98"/>
-      <c r="AD4" s="98"/>
-      <c r="AE4" s="98"/>
-      <c r="AF4" s="98"/>
-      <c r="AG4" s="98"/>
-      <c r="AH4" s="98"/>
-      <c r="AI4" s="98"/>
-      <c r="AJ4" s="98"/>
-      <c r="AK4" s="98"/>
-      <c r="AL4" s="99"/>
+      <c r="AC4" s="101"/>
+      <c r="AD4" s="101"/>
+      <c r="AE4" s="101"/>
+      <c r="AF4" s="101"/>
+      <c r="AG4" s="101"/>
+      <c r="AH4" s="101"/>
+      <c r="AI4" s="101"/>
+      <c r="AJ4" s="101"/>
+      <c r="AK4" s="101"/>
+      <c r="AL4" s="102"/>
     </row>
     <row r="5" spans="1:38" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="100"/>
-      <c r="J5" s="100"/>
-      <c r="K5" s="100"/>
-      <c r="L5" s="100"/>
-      <c r="M5" s="100"/>
-      <c r="N5" s="100"/>
-      <c r="O5" s="100"/>
-      <c r="P5" s="100"/>
-      <c r="Q5" s="100"/>
-      <c r="R5" s="100"/>
-      <c r="S5" s="100"/>
-      <c r="T5" s="100"/>
-      <c r="U5" s="100"/>
-      <c r="V5" s="100"/>
-      <c r="W5" s="100"/>
-      <c r="X5" s="100"/>
-      <c r="Y5" s="100"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="103"/>
+      <c r="F5" s="103"/>
+      <c r="G5" s="103"/>
+      <c r="H5" s="103"/>
+      <c r="I5" s="103"/>
+      <c r="J5" s="103"/>
+      <c r="K5" s="103"/>
+      <c r="L5" s="103"/>
+      <c r="M5" s="103"/>
+      <c r="N5" s="103"/>
+      <c r="O5" s="103"/>
+      <c r="P5" s="103"/>
+      <c r="Q5" s="103"/>
+      <c r="R5" s="103"/>
+      <c r="S5" s="103"/>
+      <c r="T5" s="103"/>
+      <c r="U5" s="103"/>
+      <c r="V5" s="103"/>
+      <c r="W5" s="103"/>
+      <c r="X5" s="103"/>
+      <c r="Y5" s="103"/>
       <c r="Z5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="AA5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AB5" s="92" t="s">
+      <c r="AB5" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="AC5" s="93"/>
-      <c r="AD5" s="93"/>
-      <c r="AE5" s="93"/>
-      <c r="AF5" s="93"/>
-      <c r="AG5" s="93"/>
-      <c r="AH5" s="93"/>
-      <c r="AI5" s="93"/>
-      <c r="AJ5" s="93"/>
-      <c r="AK5" s="93"/>
-      <c r="AL5" s="94"/>
+      <c r="AC5" s="96"/>
+      <c r="AD5" s="96"/>
+      <c r="AE5" s="96"/>
+      <c r="AF5" s="96"/>
+      <c r="AG5" s="96"/>
+      <c r="AH5" s="96"/>
+      <c r="AI5" s="96"/>
+      <c r="AJ5" s="96"/>
+      <c r="AK5" s="96"/>
+      <c r="AL5" s="97"/>
     </row>
     <row r="6" spans="1:38" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="92" t="s">
+      <c r="B6" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="93"/>
-      <c r="D6" s="94"/>
-      <c r="E6" s="92" t="s">
+      <c r="C6" s="96"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="93"/>
-      <c r="G6" s="94"/>
-      <c r="H6" s="92" t="s">
+      <c r="F6" s="96"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="93"/>
-      <c r="J6" s="94"/>
-      <c r="K6" s="92" t="s">
+      <c r="I6" s="96"/>
+      <c r="J6" s="97"/>
+      <c r="K6" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="93"/>
-      <c r="M6" s="94"/>
-      <c r="N6" s="92" t="s">
+      <c r="L6" s="96"/>
+      <c r="M6" s="97"/>
+      <c r="N6" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="93"/>
-      <c r="P6" s="94"/>
-      <c r="Q6" s="92" t="s">
+      <c r="O6" s="96"/>
+      <c r="P6" s="97"/>
+      <c r="Q6" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="R6" s="93"/>
-      <c r="S6" s="94"/>
-      <c r="T6" s="92" t="s">
+      <c r="R6" s="96"/>
+      <c r="S6" s="97"/>
+      <c r="T6" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="U6" s="93"/>
-      <c r="V6" s="94"/>
-      <c r="W6" s="92" t="s">
+      <c r="U6" s="96"/>
+      <c r="V6" s="97"/>
+      <c r="W6" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="X6" s="93"/>
-      <c r="Y6" s="94"/>
+      <c r="X6" s="96"/>
+      <c r="Y6" s="97"/>
       <c r="Z6" s="4" t="s">
         <v>20</v>
       </c>
@@ -1672,46 +1706,46 @@
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="93"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="92" t="s">
+      <c r="C7" s="96"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="93"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="92" t="s">
+      <c r="F7" s="96"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="93"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="92" t="s">
+      <c r="I7" s="96"/>
+      <c r="J7" s="97"/>
+      <c r="K7" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="93"/>
-      <c r="M7" s="94"/>
-      <c r="N7" s="92" t="s">
+      <c r="L7" s="96"/>
+      <c r="M7" s="97"/>
+      <c r="N7" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="93"/>
-      <c r="P7" s="94"/>
-      <c r="Q7" s="92" t="s">
+      <c r="O7" s="96"/>
+      <c r="P7" s="97"/>
+      <c r="Q7" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="R7" s="93"/>
-      <c r="S7" s="94"/>
-      <c r="T7" s="92" t="s">
+      <c r="R7" s="96"/>
+      <c r="S7" s="97"/>
+      <c r="T7" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="U7" s="93"/>
-      <c r="V7" s="94"/>
-      <c r="W7" s="92" t="s">
+      <c r="U7" s="96"/>
+      <c r="V7" s="97"/>
+      <c r="W7" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="X7" s="93"/>
-      <c r="Y7" s="94"/>
+      <c r="X7" s="96"/>
+      <c r="Y7" s="97"/>
       <c r="Z7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1756,53 +1790,53 @@
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="100" t="s">
+      <c r="B8" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="100"/>
-      <c r="D8" s="100"/>
-      <c r="E8" s="100"/>
-      <c r="F8" s="100"/>
-      <c r="G8" s="100"/>
-      <c r="H8" s="100"/>
-      <c r="I8" s="100"/>
-      <c r="J8" s="100"/>
-      <c r="K8" s="100"/>
-      <c r="L8" s="100"/>
-      <c r="M8" s="100"/>
-      <c r="N8" s="100"/>
-      <c r="O8" s="100"/>
-      <c r="P8" s="100"/>
-      <c r="Q8" s="100"/>
-      <c r="R8" s="100"/>
-      <c r="S8" s="100"/>
-      <c r="T8" s="100"/>
-      <c r="U8" s="100"/>
-      <c r="V8" s="100"/>
-      <c r="W8" s="94" t="s">
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="103"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="103"/>
+      <c r="K8" s="103"/>
+      <c r="L8" s="103"/>
+      <c r="M8" s="103"/>
+      <c r="N8" s="103"/>
+      <c r="O8" s="103"/>
+      <c r="P8" s="103"/>
+      <c r="Q8" s="103"/>
+      <c r="R8" s="103"/>
+      <c r="S8" s="103"/>
+      <c r="T8" s="103"/>
+      <c r="U8" s="103"/>
+      <c r="V8" s="103"/>
+      <c r="W8" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="X8" s="100"/>
-      <c r="Y8" s="100"/>
+      <c r="X8" s="103"/>
+      <c r="Y8" s="103"/>
       <c r="Z8" s="2" t="s">
         <v>28</v>
       </c>
       <c r="AA8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AB8" s="92" t="s">
+      <c r="AB8" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="AC8" s="93"/>
-      <c r="AD8" s="93"/>
-      <c r="AE8" s="93"/>
-      <c r="AF8" s="93"/>
-      <c r="AG8" s="93"/>
-      <c r="AH8" s="93"/>
-      <c r="AI8" s="93"/>
-      <c r="AJ8" s="93"/>
-      <c r="AK8" s="93"/>
-      <c r="AL8" s="94"/>
+      <c r="AC8" s="96"/>
+      <c r="AD8" s="96"/>
+      <c r="AE8" s="96"/>
+      <c r="AF8" s="96"/>
+      <c r="AG8" s="96"/>
+      <c r="AH8" s="96"/>
+      <c r="AI8" s="96"/>
+      <c r="AJ8" s="96"/>
+      <c r="AK8" s="96"/>
+      <c r="AL8" s="97"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
@@ -1886,19 +1920,19 @@
       <c r="AA9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AB9" s="101" t="s">
+      <c r="AB9" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="AC9" s="102"/>
-      <c r="AD9" s="102"/>
-      <c r="AE9" s="102"/>
-      <c r="AF9" s="102"/>
-      <c r="AG9" s="102"/>
-      <c r="AH9" s="102"/>
-      <c r="AI9" s="102"/>
-      <c r="AJ9" s="102"/>
-      <c r="AK9" s="102"/>
-      <c r="AL9" s="103"/>
+      <c r="AC9" s="105"/>
+      <c r="AD9" s="105"/>
+      <c r="AE9" s="105"/>
+      <c r="AF9" s="105"/>
+      <c r="AG9" s="105"/>
+      <c r="AH9" s="105"/>
+      <c r="AI9" s="105"/>
+      <c r="AJ9" s="105"/>
+      <c r="AK9" s="105"/>
+      <c r="AL9" s="106"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -2824,7 +2858,7 @@
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A16">
-        <f t="shared" si="2"/>
+        <f>A15+1</f>
         <v>22</v>
       </c>
       <c r="B16" s="6">
@@ -9642,10 +9676,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9654,11 +9688,11 @@
       <c r="A1" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="109" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
       <c r="E1" s="13" t="s">
         <v>34</v>
       </c>
@@ -9670,14 +9704,14 @@
       <c r="A2" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="109" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104" t="s">
+      <c r="C2" s="109"/>
+      <c r="D2" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="104"/>
+      <c r="E2" s="109"/>
       <c r="F2" s="13" t="s">
         <v>38</v>
       </c>
@@ -9689,24 +9723,24 @@
       <c r="B3" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="104" t="s">
+      <c r="C3" s="109" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="109" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="104"/>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
-      <c r="F4" s="104"/>
+      <c r="C4" s="109"/>
+      <c r="D4" s="109"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14">
@@ -9788,8 +9822,135 @@
         <v>20</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="92" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="107" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="107"/>
+      <c r="D13" s="93" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="93" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="108" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="92" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="108" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="108"/>
+      <c r="D14" s="108"/>
+      <c r="E14" s="93" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="108"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="92" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="108"/>
+      <c r="C15" s="108"/>
+      <c r="D15" s="108"/>
+      <c r="E15" s="93" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="108"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="94">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="94">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>9</v>
+      </c>
+      <c r="F17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="94">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <v>13</v>
+      </c>
+      <c r="E18">
+        <v>14</v>
+      </c>
+      <c r="F18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="94">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <v>19</v>
+      </c>
+      <c r="F19">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:D15"/>
+    <mergeCell ref="F13:F15"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -9805,7 +9966,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9836,11 +9997,11 @@
         <v>49</v>
       </c>
       <c r="E2" s="19"/>
-      <c r="F2" s="111" t="s">
+      <c r="F2" s="116" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
       <c r="I2" s="33" t="s">
         <v>34</v>
       </c>
@@ -9857,14 +10018,14 @@
         <v>50</v>
       </c>
       <c r="E3" s="19"/>
-      <c r="F3" s="113" t="s">
+      <c r="F3" s="118" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114" t="s">
+      <c r="G3" s="119"/>
+      <c r="H3" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="114"/>
+      <c r="I3" s="119"/>
       <c r="J3" s="35" t="s">
         <v>38</v>
       </c>
@@ -9881,12 +10042,12 @@
       <c r="F4" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="114" t="s">
+      <c r="G4" s="119" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="114"/>
-      <c r="I4" s="114"/>
-      <c r="J4" s="115"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
+      <c r="J4" s="120"/>
       <c r="K4" s="18"/>
     </row>
     <row r="5" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -9897,13 +10058,13 @@
         <v>52</v>
       </c>
       <c r="E5" s="19"/>
-      <c r="F5" s="116" t="s">
+      <c r="F5" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="117"/>
-      <c r="H5" s="117"/>
-      <c r="I5" s="117"/>
-      <c r="J5" s="118"/>
+      <c r="G5" s="122"/>
+      <c r="H5" s="122"/>
+      <c r="I5" s="122"/>
+      <c r="J5" s="123"/>
       <c r="K5" s="18"/>
     </row>
     <row r="6" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -9930,7 +10091,7 @@
       <c r="B7" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="107" t="s">
+      <c r="C7" s="112" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="38">
@@ -9956,10 +10117,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="18"/>
-      <c r="B8" s="105" t="s">
+      <c r="B8" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="108"/>
+      <c r="C8" s="113"/>
       <c r="D8" s="39">
         <v>2</v>
       </c>
@@ -9983,8 +10144,8 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="18"/>
-      <c r="B9" s="106"/>
-      <c r="C9" s="109" t="s">
+      <c r="B9" s="111"/>
+      <c r="C9" s="114" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="39">
@@ -10013,7 +10174,7 @@
       <c r="B10" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="110"/>
+      <c r="C10" s="115"/>
       <c r="D10" s="41">
         <v>4</v>
       </c>
@@ -10088,22 +10249,22 @@
       <c r="P4" s="75"/>
     </row>
     <row r="5" spans="3:16" x14ac:dyDescent="0.2">
-      <c r="C5" s="119" t="s">
+      <c r="C5" s="124" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="120"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="120"/>
-      <c r="G5" s="120"/>
-      <c r="H5" s="120"/>
-      <c r="I5" s="121"/>
-      <c r="L5" s="119" t="s">
+      <c r="D5" s="125"/>
+      <c r="E5" s="125"/>
+      <c r="F5" s="125"/>
+      <c r="G5" s="125"/>
+      <c r="H5" s="125"/>
+      <c r="I5" s="126"/>
+      <c r="L5" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="M5" s="120"/>
-      <c r="N5" s="120"/>
-      <c r="O5" s="120"/>
-      <c r="P5" s="121"/>
+      <c r="M5" s="125"/>
+      <c r="N5" s="125"/>
+      <c r="O5" s="125"/>
+      <c r="P5" s="126"/>
     </row>
     <row r="6" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C6" s="76"/>

</xml_diff>

<commit_message>
refactored so that the table definitions can be defined in the spreadsheets themselves.
</commit_message>
<xml_diff>
--- a/src/main/resources/workbooks/Testing.xlsx
+++ b/src/main/resources/workbooks/Testing.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19560" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Test1" sheetId="1" r:id="rId1"/>
-    <sheet name="Test2" sheetId="2" r:id="rId2"/>
-    <sheet name="POC" sheetId="3" r:id="rId3"/>
+    <sheet name="Definitions" sheetId="5" r:id="rId1"/>
+    <sheet name="Test1" sheetId="1" r:id="rId2"/>
+    <sheet name="Test2" sheetId="2" r:id="rId3"/>
     <sheet name="Test3" sheetId="4" r:id="rId4"/>
+    <sheet name="POC" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="93">
   <si>
     <t>Policy Number</t>
   </si>
@@ -259,6 +260,57 @@
   <si>
     <t>E:15</t>
   </si>
+  <si>
+    <t>Identification</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Column Values</t>
+  </si>
+  <si>
+    <t>Row Values</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Columns</t>
+  </si>
+  <si>
+    <t>Rows</t>
+  </si>
+  <si>
+    <t>Test 1</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>Test3 - DEATH AND TPD</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>Test3 - INCOME PROTECTION</t>
+  </si>
 </sst>
 </file>
 
@@ -334,7 +386,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -785,11 +837,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1028,6 +1117,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1041,18 +1142,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1113,6 +1202,37 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1392,6 +1512,410 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:I30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="32.5" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B2" s="127" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="128"/>
+      <c r="D2" s="127" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="128"/>
+      <c r="F2" s="127" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="128"/>
+      <c r="H2" s="129" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" s="128"/>
+    </row>
+    <row r="3" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="130" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="131" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="130" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="131" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="130" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="131" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="132" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3" s="131" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="137" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="25">
+        <v>1</v>
+      </c>
+      <c r="E4" s="24">
+        <v>2</v>
+      </c>
+      <c r="F4" s="25">
+        <v>36</v>
+      </c>
+      <c r="G4" s="24">
+        <v>8</v>
+      </c>
+      <c r="H4" s="25">
+        <v>1</v>
+      </c>
+      <c r="I4" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="138" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="17">
+        <v>1</v>
+      </c>
+      <c r="E5" s="16">
+        <v>1</v>
+      </c>
+      <c r="F5" s="17">
+        <v>5</v>
+      </c>
+      <c r="G5" s="16">
+        <v>4</v>
+      </c>
+      <c r="H5" s="17">
+        <v>1</v>
+      </c>
+      <c r="I5" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="138" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="17">
+        <v>3</v>
+      </c>
+      <c r="E6" s="16">
+        <v>7</v>
+      </c>
+      <c r="F6" s="17">
+        <v>6</v>
+      </c>
+      <c r="G6" s="16">
+        <v>3</v>
+      </c>
+      <c r="H6" s="17">
+        <v>1</v>
+      </c>
+      <c r="I6" s="28">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="138" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="17">
+        <v>12</v>
+      </c>
+      <c r="E7" s="16">
+        <v>7</v>
+      </c>
+      <c r="F7" s="17">
+        <v>4</v>
+      </c>
+      <c r="G7" s="16">
+        <v>2</v>
+      </c>
+      <c r="H7" s="17">
+        <v>1</v>
+      </c>
+      <c r="I7" s="28">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="138"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="28"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="138"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="28"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="138"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="28"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="138"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="28"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="138"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="28"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="138"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="28"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="138"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="28"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="138"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="78"/>
+      <c r="H15" s="77"/>
+      <c r="I15" s="134"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="138"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="77"/>
+      <c r="I16" s="134"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="138"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="77"/>
+      <c r="I17" s="134"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" s="138"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="77"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="77"/>
+      <c r="G18" s="78"/>
+      <c r="H18" s="77"/>
+      <c r="I18" s="134"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19" s="138"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="77"/>
+      <c r="I19" s="134"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" s="138"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="77"/>
+      <c r="I20" s="134"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" s="138"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="78"/>
+      <c r="H21" s="77"/>
+      <c r="I21" s="134"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="138"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="78"/>
+      <c r="H22" s="77"/>
+      <c r="I22" s="134"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="138"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="77"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="77"/>
+      <c r="I23" s="134"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="138"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="77"/>
+      <c r="E24" s="78"/>
+      <c r="F24" s="77"/>
+      <c r="G24" s="78"/>
+      <c r="H24" s="77"/>
+      <c r="I24" s="134"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="138"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="77"/>
+      <c r="I25" s="134"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="138"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="77"/>
+      <c r="I26" s="134"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="138"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="77"/>
+      <c r="I27" s="134"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" s="138"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="77"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="77"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="77"/>
+      <c r="I28" s="134"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" s="138"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="77"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="78"/>
+      <c r="H29" s="77"/>
+      <c r="I29" s="134"/>
+    </row>
+    <row r="30" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="139"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="135"/>
+      <c r="E30" s="133"/>
+      <c r="F30" s="135"/>
+      <c r="G30" s="133"/>
+      <c r="H30" s="135"/>
+      <c r="I30" s="136"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1458,32 +1982,32 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="98">
+      <c r="B3" s="102">
         <v>1</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
-      <c r="Q3" s="98"/>
-      <c r="R3" s="98"/>
-      <c r="S3" s="98"/>
-      <c r="T3" s="98"/>
-      <c r="U3" s="98"/>
-      <c r="V3" s="98"/>
-      <c r="W3" s="98"/>
-      <c r="X3" s="98"/>
-      <c r="Y3" s="98"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="102"/>
+      <c r="L3" s="102"/>
+      <c r="M3" s="102"/>
+      <c r="N3" s="102"/>
+      <c r="O3" s="102"/>
+      <c r="P3" s="102"/>
+      <c r="Q3" s="102"/>
+      <c r="R3" s="102"/>
+      <c r="S3" s="102"/>
+      <c r="T3" s="102"/>
+      <c r="U3" s="102"/>
+      <c r="V3" s="102"/>
+      <c r="W3" s="102"/>
+      <c r="X3" s="102"/>
+      <c r="Y3" s="102"/>
       <c r="Z3" s="2">
         <v>2</v>
       </c>
@@ -1508,96 +2032,96 @@
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="99" t="s">
+      <c r="B4" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99" t="s">
+      <c r="C4" s="103"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99" t="s">
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
-      <c r="K4" s="99" t="s">
+      <c r="I4" s="103"/>
+      <c r="J4" s="103"/>
+      <c r="K4" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="99"/>
-      <c r="M4" s="99"/>
-      <c r="N4" s="99" t="s">
+      <c r="L4" s="103"/>
+      <c r="M4" s="103"/>
+      <c r="N4" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="99"/>
-      <c r="P4" s="99"/>
-      <c r="Q4" s="99" t="s">
+      <c r="O4" s="103"/>
+      <c r="P4" s="103"/>
+      <c r="Q4" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="R4" s="99"/>
-      <c r="S4" s="99"/>
-      <c r="T4" s="99" t="s">
+      <c r="R4" s="103"/>
+      <c r="S4" s="103"/>
+      <c r="T4" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="U4" s="99"/>
-      <c r="V4" s="99"/>
-      <c r="W4" s="100" t="s">
+      <c r="U4" s="103"/>
+      <c r="V4" s="103"/>
+      <c r="W4" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="X4" s="101"/>
-      <c r="Y4" s="102"/>
+      <c r="X4" s="105"/>
+      <c r="Y4" s="106"/>
       <c r="Z4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="AA4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="100" t="s">
+      <c r="AB4" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="AC4" s="101"/>
-      <c r="AD4" s="101"/>
-      <c r="AE4" s="101"/>
-      <c r="AF4" s="101"/>
-      <c r="AG4" s="101"/>
-      <c r="AH4" s="101"/>
-      <c r="AI4" s="101"/>
-      <c r="AJ4" s="101"/>
-      <c r="AK4" s="101"/>
-      <c r="AL4" s="102"/>
+      <c r="AC4" s="105"/>
+      <c r="AD4" s="105"/>
+      <c r="AE4" s="105"/>
+      <c r="AF4" s="105"/>
+      <c r="AG4" s="105"/>
+      <c r="AH4" s="105"/>
+      <c r="AI4" s="105"/>
+      <c r="AJ4" s="105"/>
+      <c r="AK4" s="105"/>
+      <c r="AL4" s="106"/>
     </row>
     <row r="5" spans="1:38" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="103" t="s">
+      <c r="B5" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
-      <c r="E5" s="103"/>
-      <c r="F5" s="103"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="103"/>
-      <c r="J5" s="103"/>
-      <c r="K5" s="103"/>
-      <c r="L5" s="103"/>
-      <c r="M5" s="103"/>
-      <c r="N5" s="103"/>
-      <c r="O5" s="103"/>
-      <c r="P5" s="103"/>
-      <c r="Q5" s="103"/>
-      <c r="R5" s="103"/>
-      <c r="S5" s="103"/>
-      <c r="T5" s="103"/>
-      <c r="U5" s="103"/>
-      <c r="V5" s="103"/>
-      <c r="W5" s="103"/>
-      <c r="X5" s="103"/>
-      <c r="Y5" s="103"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="98"/>
+      <c r="P5" s="98"/>
+      <c r="Q5" s="98"/>
+      <c r="R5" s="98"/>
+      <c r="S5" s="98"/>
+      <c r="T5" s="98"/>
+      <c r="U5" s="98"/>
+      <c r="V5" s="98"/>
+      <c r="W5" s="98"/>
+      <c r="X5" s="98"/>
+      <c r="Y5" s="98"/>
       <c r="Z5" s="4" t="s">
         <v>17</v>
       </c>
@@ -1790,34 +2314,34 @@
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="103"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="103"/>
-      <c r="F8" s="103"/>
-      <c r="G8" s="103"/>
-      <c r="H8" s="103"/>
-      <c r="I8" s="103"/>
-      <c r="J8" s="103"/>
-      <c r="K8" s="103"/>
-      <c r="L8" s="103"/>
-      <c r="M8" s="103"/>
-      <c r="N8" s="103"/>
-      <c r="O8" s="103"/>
-      <c r="P8" s="103"/>
-      <c r="Q8" s="103"/>
-      <c r="R8" s="103"/>
-      <c r="S8" s="103"/>
-      <c r="T8" s="103"/>
-      <c r="U8" s="103"/>
-      <c r="V8" s="103"/>
+      <c r="C8" s="98"/>
+      <c r="D8" s="98"/>
+      <c r="E8" s="98"/>
+      <c r="F8" s="98"/>
+      <c r="G8" s="98"/>
+      <c r="H8" s="98"/>
+      <c r="I8" s="98"/>
+      <c r="J8" s="98"/>
+      <c r="K8" s="98"/>
+      <c r="L8" s="98"/>
+      <c r="M8" s="98"/>
+      <c r="N8" s="98"/>
+      <c r="O8" s="98"/>
+      <c r="P8" s="98"/>
+      <c r="Q8" s="98"/>
+      <c r="R8" s="98"/>
+      <c r="S8" s="98"/>
+      <c r="T8" s="98"/>
+      <c r="U8" s="98"/>
+      <c r="V8" s="98"/>
       <c r="W8" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="X8" s="103"/>
-      <c r="Y8" s="103"/>
+      <c r="X8" s="98"/>
+      <c r="Y8" s="98"/>
       <c r="Z8" s="2" t="s">
         <v>28</v>
       </c>
@@ -1920,19 +2444,19 @@
       <c r="AA9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AB9" s="104" t="s">
+      <c r="AB9" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="AC9" s="105"/>
-      <c r="AD9" s="105"/>
-      <c r="AE9" s="105"/>
-      <c r="AF9" s="105"/>
-      <c r="AG9" s="105"/>
-      <c r="AH9" s="105"/>
-      <c r="AI9" s="105"/>
-      <c r="AJ9" s="105"/>
-      <c r="AK9" s="105"/>
-      <c r="AL9" s="106"/>
+      <c r="AC9" s="100"/>
+      <c r="AD9" s="100"/>
+      <c r="AE9" s="100"/>
+      <c r="AF9" s="100"/>
+      <c r="AG9" s="100"/>
+      <c r="AH9" s="100"/>
+      <c r="AI9" s="100"/>
+      <c r="AJ9" s="100"/>
+      <c r="AK9" s="100"/>
+      <c r="AL9" s="101"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -9634,28 +10158,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="W7:Y7"/>
-    <mergeCell ref="B8:V8"/>
-    <mergeCell ref="W8:Y8"/>
-    <mergeCell ref="AB8:AL8"/>
-    <mergeCell ref="AB9:AL9"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="T7:V7"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="B5:Y5"/>
-    <mergeCell ref="AB5:AL5"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="T6:V6"/>
-    <mergeCell ref="W6:Y6"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N6:P6"/>
     <mergeCell ref="B2:Z2"/>
     <mergeCell ref="AA2:AL2"/>
     <mergeCell ref="B3:Y3"/>
@@ -9669,17 +10171,39 @@
     <mergeCell ref="T4:V4"/>
     <mergeCell ref="W4:Y4"/>
     <mergeCell ref="AB4:AL4"/>
+    <mergeCell ref="B5:Y5"/>
+    <mergeCell ref="AB5:AL5"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="T6:V6"/>
+    <mergeCell ref="W6:Y6"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="W7:Y7"/>
+    <mergeCell ref="B8:V8"/>
+    <mergeCell ref="W8:Y8"/>
+    <mergeCell ref="AB8:AL8"/>
+    <mergeCell ref="AB9:AL9"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="T7:V7"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="N7:P7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9956,269 +10480,6 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="B4:F4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="5" max="5" width="2" customWidth="1"/>
-    <col min="11" max="11" width="2.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="116" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="18"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="118" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="119"/>
-      <c r="H3" s="119" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="119"/>
-      <c r="J3" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" s="18"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="119" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
-      <c r="J4" s="120"/>
-      <c r="K4" s="18"/>
-    </row>
-    <row r="5" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="121" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" s="122"/>
-      <c r="H5" s="122"/>
-      <c r="I5" s="122"/>
-      <c r="J5" s="123"/>
-      <c r="K5" s="18"/>
-    </row>
-    <row r="6" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="18"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
-      <c r="B7" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="112" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="38">
-        <v>1</v>
-      </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="23">
-        <v>1</v>
-      </c>
-      <c r="G7" s="24">
-        <v>2</v>
-      </c>
-      <c r="H7" s="25">
-        <v>3</v>
-      </c>
-      <c r="I7" s="24">
-        <v>4</v>
-      </c>
-      <c r="J7" s="26">
-        <v>5</v>
-      </c>
-      <c r="K7" s="18"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
-      <c r="B8" s="110" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="113"/>
-      <c r="D8" s="39">
-        <v>2</v>
-      </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="27">
-        <v>6</v>
-      </c>
-      <c r="G8" s="16">
-        <v>7</v>
-      </c>
-      <c r="H8" s="17">
-        <v>8</v>
-      </c>
-      <c r="I8" s="16">
-        <v>9</v>
-      </c>
-      <c r="J8" s="28">
-        <v>10</v>
-      </c>
-      <c r="K8" s="18"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
-      <c r="B9" s="111"/>
-      <c r="C9" s="114" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="39">
-        <v>3</v>
-      </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="27">
-        <v>11</v>
-      </c>
-      <c r="G9" s="16">
-        <v>12</v>
-      </c>
-      <c r="H9" s="17">
-        <v>13</v>
-      </c>
-      <c r="I9" s="16">
-        <v>14</v>
-      </c>
-      <c r="J9" s="28">
-        <v>15</v>
-      </c>
-      <c r="K9" s="18"/>
-    </row>
-    <row r="10" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="115"/>
-      <c r="D10" s="41">
-        <v>4</v>
-      </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="29">
-        <v>16</v>
-      </c>
-      <c r="G10" s="30">
-        <v>17</v>
-      </c>
-      <c r="H10" s="31">
-        <v>18</v>
-      </c>
-      <c r="I10" s="30">
-        <v>19</v>
-      </c>
-      <c r="J10" s="32">
-        <v>20</v>
-      </c>
-      <c r="K10" s="18"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-    </row>
-  </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="F5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12879,4 +13140,267 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="5" max="5" width="2" customWidth="1"/>
+    <col min="11" max="11" width="2.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="19"/>
+      <c r="F2" s="116" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="18"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="19"/>
+      <c r="F3" s="118" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="119"/>
+      <c r="H3" s="119" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="119"/>
+      <c r="J3" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="18"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="19"/>
+      <c r="F4" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="119" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
+      <c r="J4" s="120"/>
+      <c r="K4" s="18"/>
+    </row>
+    <row r="5" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="19"/>
+      <c r="F5" s="121" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="122"/>
+      <c r="H5" s="122"/>
+      <c r="I5" s="122"/>
+      <c r="J5" s="123"/>
+      <c r="K5" s="18"/>
+    </row>
+    <row r="6" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="18"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="18"/>
+      <c r="B7" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="112" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="38">
+        <v>1</v>
+      </c>
+      <c r="E7" s="21"/>
+      <c r="F7" s="23">
+        <v>1</v>
+      </c>
+      <c r="G7" s="24">
+        <v>2</v>
+      </c>
+      <c r="H7" s="25">
+        <v>3</v>
+      </c>
+      <c r="I7" s="24">
+        <v>4</v>
+      </c>
+      <c r="J7" s="26">
+        <v>5</v>
+      </c>
+      <c r="K7" s="18"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="18"/>
+      <c r="B8" s="110" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="113"/>
+      <c r="D8" s="39">
+        <v>2</v>
+      </c>
+      <c r="E8" s="21"/>
+      <c r="F8" s="27">
+        <v>6</v>
+      </c>
+      <c r="G8" s="16">
+        <v>7</v>
+      </c>
+      <c r="H8" s="17">
+        <v>8</v>
+      </c>
+      <c r="I8" s="16">
+        <v>9</v>
+      </c>
+      <c r="J8" s="28">
+        <v>10</v>
+      </c>
+      <c r="K8" s="18"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="18"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="114" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="39">
+        <v>3</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="27">
+        <v>11</v>
+      </c>
+      <c r="G9" s="16">
+        <v>12</v>
+      </c>
+      <c r="H9" s="17">
+        <v>13</v>
+      </c>
+      <c r="I9" s="16">
+        <v>14</v>
+      </c>
+      <c r="J9" s="28">
+        <v>15</v>
+      </c>
+      <c r="K9" s="18"/>
+    </row>
+    <row r="10" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="115"/>
+      <c r="D10" s="41">
+        <v>4</v>
+      </c>
+      <c r="E10" s="21"/>
+      <c r="F10" s="29">
+        <v>16</v>
+      </c>
+      <c r="G10" s="30">
+        <v>17</v>
+      </c>
+      <c r="H10" s="31">
+        <v>18</v>
+      </c>
+      <c r="I10" s="30">
+        <v>19</v>
+      </c>
+      <c r="J10" s="32">
+        <v>20</v>
+      </c>
+      <c r="K10" s="18"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="F5:J5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added support for getting a tree of valid options.
</commit_message>
<xml_diff>
--- a/src/main/resources/workbooks/Testing.xlsx
+++ b/src/main/resources/workbooks/Testing.xlsx
@@ -1515,7 +1515,7 @@
   <dimension ref="B1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1592,7 +1592,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="26">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
@@ -1918,8 +1918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AB9" sqref="AB9:AL9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>